<commit_message>
added lv power cable
</commit_message>
<xml_diff>
--- a/data/Polycab/Cables/LV Power Cables/scripts/polycab_lv_power_cable/polycab_lv_power_cable_complete.xlsx
+++ b/data/Polycab/Cables/LV Power Cables/scripts/polycab_lv_power_cable/polycab_lv_power_cable_complete.xlsx
@@ -435,13 +435,13 @@
   <cols>
     <col width="46" customWidth="1" min="1" max="1"/>
     <col width="16" customWidth="1" min="2" max="2"/>
-    <col width="33" customWidth="1" min="3" max="3"/>
+    <col width="13" customWidth="1" min="3" max="3"/>
     <col width="20" customWidth="1" min="4" max="4"/>
-    <col width="25" customWidth="1" min="5" max="5"/>
+    <col width="50" customWidth="1" min="5" max="5"/>
     <col width="50" customWidth="1" min="6" max="6"/>
     <col width="50" customWidth="1" min="7" max="7"/>
     <col width="50" customWidth="1" min="8" max="8"/>
-    <col width="12" customWidth="1" min="9" max="9"/>
+    <col width="50" customWidth="1" min="9" max="9"/>
     <col width="50" customWidth="1" min="10" max="10"/>
     <col width="23" customWidth="1" min="11" max="11"/>
     <col width="26" customWidth="1" min="12" max="12"/>
@@ -512,7 +512,7 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>Polycab LV IS-7098-I 2C A2XWY</t>
+          <t>Polycab LV IS-7098-I 1C-2XY</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
@@ -522,7 +522,7 @@
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>IEC 60502-1, IS 7098-1, BS 5467</t>
+          <t>IS 7098-I</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
@@ -530,23 +530,39 @@
           <t>CE, BIS, CPRI, FQC</t>
         </is>
       </c>
-      <c r="E2" t="inlineStr"/>
-      <c r="F2" t="inlineStr"/>
-      <c r="G2" t="inlineStr"/>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>Higher Current rating, Higher insulation resistance, Better resistance to surge current, Low dielectric losses, Long service life, Higher short circuit rating</t>
+        </is>
+      </c>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>Single core Copper, XLPE Insulation , unarmoured &amp; PVC Outer sheathed cable</t>
+        </is>
+      </c>
+      <c r="G2" t="inlineStr">
+        <is>
+          <t>POLYCAB 2XY SC, stranded compacted copper conductor, XLPE insulated and PVC sheathed confirming to IS 7098-1 is suitable for AC single phase or three phase (earthed or unearthed) systems with rated voltage up to and including 1100 V. This cable is also suitable for DC systems with rated voltage up to and including 1500 V</t>
+        </is>
+      </c>
       <c r="H2" t="inlineStr">
         <is>
-          <t>https://polycab.com/polycab-lv-is-7098-i-2c-a2xwy/pt-13191/p-54706</t>
-        </is>
-      </c>
-      <c r="I2" t="inlineStr"/>
+          <t>https://polycab.com/polycab-lv-is-7098-i-1c-2xy/pt-13191/p-54736</t>
+        </is>
+      </c>
+      <c r="I2" t="inlineStr">
+        <is>
+          <t>polycab_lv_power_cable/images/Polycab_LV_IS-7098-I_1C-2XY_image.png</t>
+        </is>
+      </c>
       <c r="J2" t="inlineStr">
         <is>
-          <t>polycab_lv_power_cable/brochures/Polycab_LV_IS-7098-I_2C_A2XWY_datasheet.pdf</t>
+          <t>polycab_lv_power_cable/brochures/Polycab_LV_IS-7098-I_1C-2XY_datasheet.pdf</t>
         </is>
       </c>
       <c r="K2" t="inlineStr">
         <is>
-          <t>Not Found</t>
+          <t>Downloaded</t>
         </is>
       </c>
       <c r="L2" t="inlineStr">
@@ -558,7 +574,7 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>Polycab BS 5467 SC 0.6/1kV AC</t>
+          <t>Polycab LV AL IEC 60502-1 0.6/1kV MC-2 UA</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
@@ -568,7 +584,7 @@
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>IEC 60502-1, BS 5467</t>
+          <t>IEC 60502-1</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
@@ -578,25 +594,37 @@
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>High Life, Low Smoke</t>
-        </is>
-      </c>
-      <c r="F3" t="inlineStr"/>
-      <c r="G3" t="inlineStr"/>
+          <t>Higher dielectric strength, Better electrical, mechanical, And thermal properties, UV resistant, Long service life, Low smoke emission</t>
+        </is>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>Multi core stranded AL conductor, XLPE/EPR/HEPR insulation, Laid up, Inner covering, Armoured, PVC/Polyethylene/Halogen free Outer sheathed LV Cable</t>
+        </is>
+      </c>
+      <c r="G3" t="inlineStr">
+        <is>
+          <t>Multicore stranded Aluminium, XLPE/EPR/HEPR insulation, Laid up, inner covering,PVC/Polyethylene/Halogen free sheathed unarmored Cable suitable for fixed installation such as distribution network or industrial installation.These cables are designed for systems with rated AC voltage 1KV (Um=1.2 KV) between two live conductor.</t>
+        </is>
+      </c>
       <c r="H3" t="inlineStr">
         <is>
-          <t>https://polycab.com/polycab-bs-5467-sc-061kv-ac/pt-13191/p-55465</t>
-        </is>
-      </c>
-      <c r="I3" t="inlineStr"/>
+          <t>https://polycab.com/polycab-lv-al-iec-60502-1-061kv-mc-2-ua/pt-13191/p-55259</t>
+        </is>
+      </c>
+      <c r="I3" t="inlineStr">
+        <is>
+          <t>polycab_lv_power_cable/images/Polycab_LV_AL_IEC_60502-1_061kV_MC-2_UA_image.png</t>
+        </is>
+      </c>
       <c r="J3" t="inlineStr">
         <is>
-          <t>polycab_lv_power_cable/brochures/Polycab_BS_5467_SC_061kV_AC_datasheet.pdf</t>
+          <t>polycab_lv_power_cable/brochures/Polycab_LV_AL_IEC_60502-1_061kV_MC-2_UA_datasheet.pdf</t>
         </is>
       </c>
       <c r="K3" t="inlineStr">
         <is>
-          <t>Not Found</t>
+          <t>Downloaded</t>
         </is>
       </c>
       <c r="L3" t="inlineStr">
@@ -608,7 +636,7 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>Polycab LV AL IEC 60502-1 0.6/1kV SC UA</t>
+          <t>Polycab LV IS-7098-I 3C 2XFY</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
@@ -618,35 +646,47 @@
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>IEC 60502-1, BS 5467</t>
+          <t>IS 7098-I</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>CE, FQC</t>
+          <t>CE, BIS, CPRI, FQC</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>UV Resistant, Low Smoke</t>
-        </is>
-      </c>
-      <c r="F4" t="inlineStr"/>
-      <c r="G4" t="inlineStr"/>
+          <t>Higher Current rating, Higher insulation resistance, Better resistance to surge current, Low dielectric losses, Long service life, Higher short circuit rating</t>
+        </is>
+      </c>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>Three core copper conductor, XLPE Insulation,Inner sheathed &amp; GI flat armoured &amp; PVC Outer sheathed cable</t>
+        </is>
+      </c>
+      <c r="G4" t="inlineStr">
+        <is>
+          <t>POLYCAB 2XFY MC-3,Stranded compacted copper conductor, XLPE insulated, PVC inner sheathed, Galvanised Steel Flat strip armour and PVC sheathed confirming to IS 7098-1 is suitable for AC single phase or three phase (earthed or unearthed) systems with rated voltage up to and including 1100 V. This cable is also suitable for DC systems with rated voltage up to and including 1500 V</t>
+        </is>
+      </c>
       <c r="H4" t="inlineStr">
         <is>
-          <t>https://polycab.com/polycab-lv-al-iec-60502-1-061kv-sc-ua/pt-13191/p-55243</t>
-        </is>
-      </c>
-      <c r="I4" t="inlineStr"/>
+          <t>https://polycab.com/polycab-lv-is-7098-i-3c-2xfy/pt-13191/p-54716</t>
+        </is>
+      </c>
+      <c r="I4" t="inlineStr">
+        <is>
+          <t>polycab_lv_power_cable/images/Polycab_LV_IS-7098-I_3C_2XFY_image.png</t>
+        </is>
+      </c>
       <c r="J4" t="inlineStr">
         <is>
-          <t>polycab_lv_power_cable/brochures/Polycab_LV_AL_IEC_60502-1_061kV_SC_UA_datasheet.pdf</t>
+          <t>polycab_lv_power_cable/brochures/Polycab_LV_IS-7098-I_3C_2XFY_datasheet.pdf</t>
         </is>
       </c>
       <c r="K4" t="inlineStr">
         <is>
-          <t>Not Found</t>
+          <t>Downloaded</t>
         </is>
       </c>
       <c r="L4" t="inlineStr">
@@ -658,7 +698,7 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>Polycab LV IS-7098-I 3C 2XFY</t>
+          <t>Polycab LV IS-7098-I 3C A2XWY</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
@@ -668,7 +708,7 @@
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>IEC 60502-1, IS 7098-1, BS 5467</t>
+          <t>IS 7098-I</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
@@ -676,23 +716,39 @@
           <t>CE, BIS, CPRI, FQC</t>
         </is>
       </c>
-      <c r="E5" t="inlineStr"/>
-      <c r="F5" t="inlineStr"/>
-      <c r="G5" t="inlineStr"/>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>Higher Current rating, Higher insulation resistance, Better resistance to surge current, Low dielectric losses, Long service life, Higher short circuit rating</t>
+        </is>
+      </c>
+      <c r="F5" t="inlineStr">
+        <is>
+          <t>Three core aluminium, XLPE Insulation, Inner sheathed &amp; GI round armoured &amp; PVC Outer sheathed cable</t>
+        </is>
+      </c>
+      <c r="G5" t="inlineStr">
+        <is>
+          <t>POLYCAB A2XWY MC-3, Stranded compacted aluminium conductor, XLPE insulated, PVC inner sheathed, Galvanised Steel round wire armour and PVC sheathed confirming to IS 7098-1 is suitable for AC single phase or three phase (earthed or unearthed) systems with rated voltage up to and including 1100 V. This cable is also suitable for DC systems with rated voltage up to and including 1500 V</t>
+        </is>
+      </c>
       <c r="H5" t="inlineStr">
         <is>
-          <t>https://polycab.com/polycab-lv-is-7098-i-3c-2xfy/pt-13191/p-54716</t>
-        </is>
-      </c>
-      <c r="I5" t="inlineStr"/>
+          <t>https://polycab.com/polycab-lv-is-7098-i-3c-a2xwy/pt-13191/p-54722</t>
+        </is>
+      </c>
+      <c r="I5" t="inlineStr">
+        <is>
+          <t>polycab_lv_power_cable/images/Polycab_LV_IS-7098-I_3C_A2XWY_image.png</t>
+        </is>
+      </c>
       <c r="J5" t="inlineStr">
         <is>
-          <t>polycab_lv_power_cable/brochures/Polycab_LV_IS-7098-I_3C_2XFY_datasheet.pdf</t>
+          <t>polycab_lv_power_cable/brochures/Polycab_LV_IS-7098-I_3C_A2XWY_datasheet.pdf</t>
         </is>
       </c>
       <c r="K5" t="inlineStr">
         <is>
-          <t>Not Found</t>
+          <t>Downloaded</t>
         </is>
       </c>
       <c r="L5" t="inlineStr">
@@ -704,7 +760,7 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>Polycab LV Cu IEC 60502-1 0.6/1kV SC UA</t>
+          <t>Polycab BS 6724 MC SWA LSZH 0.6/1kV AC</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
@@ -714,7 +770,7 @@
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>IEC 60502-1, BS 5467</t>
+          <t>BS 6724</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
@@ -724,33 +780,37 @@
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>UV Resistant, Low Smoke</t>
+          <t>Low flame propagation, Low smoke emission, High life, Halogen Free</t>
         </is>
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>Single core stranded Copper conductor, XLPE/EPR/HEPR insulation,PVC/Polyethylene/Halogen free Inner &amp;amp; outer sheathed Cable. suitable for fixed installation such as distribution network or industrial installation. These cable cables are designed for systems with rated AC voltage 1KV (Um=1.2 KV).</t>
+          <t>Stranded copper conductor, XLPE/EPR/HEPR Insulated, Extruded Polymeric Bedding, GS round wire armoured, LSZH Outer Sheathed 0.6/1 kV LV cable</t>
         </is>
       </c>
       <c r="G6" t="inlineStr">
         <is>
-          <t>Single core stranded Copper conductor, XLPE/EPR/HEPR insulation,PVC/Polyethylene/Halogen free Inner &amp;amp; outer sheathed Cable. suitable for fixed installation such as distribution network or industrial installation. These cable cables are designed for systems with rated AC voltage 1KV (Um=1.2 KV).</t>
+          <t>POLYCAB BS 6724 MC SWA LSZH stranded copper conductor thermosetting material insulated Galvanised steel wire armoured multicore cable is designed to use for fixed installation in indoor and outdoor power network, underground application, industrial areas and buildings where smoke emission and toxic fumes create a potential risk when exposed to fire.</t>
         </is>
       </c>
       <c r="H6" t="inlineStr">
         <is>
-          <t>https://polycab.com/polycab-lv-cu-iec-60502-1-061kv-sc-ua/pt-13191/p-55253</t>
-        </is>
-      </c>
-      <c r="I6" t="inlineStr"/>
+          <t>https://polycab.com/polycab-bs-6724-mc-swa-lszh-061kv-ac/pt-13191/p-55457</t>
+        </is>
+      </c>
+      <c r="I6" t="inlineStr">
+        <is>
+          <t>polycab_lv_power_cable/images/Polycab_BS_6724_MC_SWA_LSZH_061kV_AC_image.png</t>
+        </is>
+      </c>
       <c r="J6" t="inlineStr">
         <is>
-          <t>polycab_lv_power_cable/brochures/Polycab_LV_Cu_IEC_60502-1_061kV_SC_UA_datasheet.pdf</t>
+          <t>polycab_lv_power_cable/brochures/Polycab_BS_6724_MC_SWA_LSZH_061kV_AC_datasheet.pdf</t>
         </is>
       </c>
       <c r="K6" t="inlineStr">
         <is>
-          <t>Not Found</t>
+          <t>Downloaded</t>
         </is>
       </c>
       <c r="L6" t="inlineStr">
@@ -762,7 +822,7 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>Polycab LV Cu IEC 60502-1 0.6/1kV MC-4 SFA</t>
+          <t>Polycab LV Cu IEC 60502-1 0.6/1kV MC-4 UA</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
@@ -772,7 +832,7 @@
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>IEC 60502-1, BS 5467</t>
+          <t>IEC 60502-1</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
@@ -782,25 +842,37 @@
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>UV Resistant, Low Smoke</t>
-        </is>
-      </c>
-      <c r="F7" t="inlineStr"/>
-      <c r="G7" t="inlineStr"/>
+          <t>Higher dielectric strength, Better electrical, mechanical, And thermal properties, UV resistant, Long service life, Low smoke emission</t>
+        </is>
+      </c>
+      <c r="F7" t="inlineStr">
+        <is>
+          <t>Multi core stranded copper conductor, XLPE insulation, Laid up, Inner covering, Armoured,PVC/Polyethylene/Halogen free Outer sheathed LV Cable</t>
+        </is>
+      </c>
+      <c r="G7" t="inlineStr">
+        <is>
+          <t>Multicore stranded Copper, XLPE/EPR/HEPR insulation, Laid up, inner covering,PVC/Polyethylene/Halogen free sheathed unarmored Cable suitable for fixed installation such as distribution network or industrial installation.These cables are designed for systems with rated AC voltage 1KV (Um=1.2 KV) between two live conductor.</t>
+        </is>
+      </c>
       <c r="H7" t="inlineStr">
         <is>
-          <t>https://polycab.com/polycab-lv-cu-iec-60502-1-061kv-mc-4-sfa/pt-13191/p-55297</t>
-        </is>
-      </c>
-      <c r="I7" t="inlineStr"/>
+          <t>https://polycab.com/polycab-lv-cu-iec-60502-1-061kv-mc-4-ua/pt-13191/p-55301</t>
+        </is>
+      </c>
+      <c r="I7" t="inlineStr">
+        <is>
+          <t>polycab_lv_power_cable/images/Polycab_LV_Cu_IEC_60502-1_061kV_MC-4_UA_image.png</t>
+        </is>
+      </c>
       <c r="J7" t="inlineStr">
         <is>
-          <t>polycab_lv_power_cable/brochures/Polycab_LV_Cu_IEC_60502-1_061kV_MC-4_SFA_datasheet.pdf</t>
+          <t>polycab_lv_power_cable/brochures/Polycab_LV_Cu_IEC_60502-1_061kV_MC-4_UA_datasheet.pdf</t>
         </is>
       </c>
       <c r="K7" t="inlineStr">
         <is>
-          <t>Not Found</t>
+          <t>Downloaded</t>
         </is>
       </c>
       <c r="L7" t="inlineStr">
@@ -812,7 +884,7 @@
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>Polycab LV Cu IEC 60502-1 0.6/1kV SC AWA</t>
+          <t>Polycab LV Cu IEC 60502-1 0.6/1kV MC-4 SWA</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
@@ -822,7 +894,7 @@
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>IEC 60502-1, BS 5467</t>
+          <t>IEC 60502-1</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
@@ -832,25 +904,37 @@
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>UV Resistant, Low Smoke</t>
-        </is>
-      </c>
-      <c r="F8" t="inlineStr"/>
-      <c r="G8" t="inlineStr"/>
+          <t>Higher dielectric strength, Better electrical, mechanical, And thermal properties, UV resistant, Long service life, Low smoke emission</t>
+        </is>
+      </c>
+      <c r="F8" t="inlineStr">
+        <is>
+          <t>Multi core stranded copper conductor,XLPE/EPR/HEPR insulation, Laid up, Inner covering, Armoured, PVC/Polyethylene/Halogen free Outer sheathed LV Cable</t>
+        </is>
+      </c>
+      <c r="G8" t="inlineStr">
+        <is>
+          <t>Multicore stranded Copper, XLPE/EPR/HEPR insulation, Laid up, inner covering,GI wire,PVC/Polyethylene/Halogen free sheathed Cable suitable for fixed installation such as distribution network or industrial installation.These cables are designed for systems with rated AC voltage 1KV (Um=1.2 KV) between two live conductor.</t>
+        </is>
+      </c>
       <c r="H8" t="inlineStr">
         <is>
-          <t>https://polycab.com/polycab-lv-cu-iec-60502-1-061kv-sc-awa/pt-13191/p-55249</t>
-        </is>
-      </c>
-      <c r="I8" t="inlineStr"/>
+          <t>https://polycab.com/polycab-lv-cu-iec-60502-1-061kv-mc-4-swa/pt-13191/p-55299</t>
+        </is>
+      </c>
+      <c r="I8" t="inlineStr">
+        <is>
+          <t>polycab_lv_power_cable/images/Polycab_LV_Cu_IEC_60502-1_061kV_MC-4_SWA_image.png</t>
+        </is>
+      </c>
       <c r="J8" t="inlineStr">
         <is>
-          <t>polycab_lv_power_cable/brochures/Polycab_LV_Cu_IEC_60502-1_061kV_SC_AWA_datasheet.pdf</t>
+          <t>polycab_lv_power_cable/brochures/Polycab_LV_Cu_IEC_60502-1_061kV_MC-4_SWA_datasheet.pdf</t>
         </is>
       </c>
       <c r="K8" t="inlineStr">
         <is>
-          <t>Not Found</t>
+          <t>Downloaded</t>
         </is>
       </c>
       <c r="L8" t="inlineStr">
@@ -862,7 +946,7 @@
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>Polycab LV Cu IEC 60502-1 0.6/1kV MC-4 SWA</t>
+          <t>Polycab LV Cu IEC 60502-1 0.6/1kV MC-3 SWA</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
@@ -872,7 +956,7 @@
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>IEC 60502-1, BS 5467</t>
+          <t>IEC 60502-1</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
@@ -882,25 +966,37 @@
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>UV Resistant, Low Smoke</t>
-        </is>
-      </c>
-      <c r="F9" t="inlineStr"/>
-      <c r="G9" t="inlineStr"/>
+          <t>Higher dielectric strength, Better electrical, mechanical, And thermal properties, UV resistant, Long service life, Low smoke emission</t>
+        </is>
+      </c>
+      <c r="F9" t="inlineStr">
+        <is>
+          <t>Multi core stranded copper conductor,XLPE/EPR/HEPR insulation, Laid up, Inner covering, Armoured, PVC/Polyethylene/Halogen free inner &amp; Outer sheathed LV Cable</t>
+        </is>
+      </c>
+      <c r="G9" t="inlineStr">
+        <is>
+          <t>Multicore stranded Copper, XLPE/EPR/HEPR insulation, Laid up, inner covering,GI wire,PVC/Polyethylene/Halogen free sheathed Cable suitable for fixed installation such as distribution network or industrial installation.These cables are designed for systems with rated AC voltage 1KV (Um=1.2 KV) between two live conductor.</t>
+        </is>
+      </c>
       <c r="H9" t="inlineStr">
         <is>
-          <t>https://polycab.com/polycab-lv-cu-iec-60502-1-061kv-mc-4-swa/pt-13191/p-55299</t>
-        </is>
-      </c>
-      <c r="I9" t="inlineStr"/>
+          <t>https://polycab.com/polycab-lv-cu-iec-60502-1-061kv-mc-3-swa/pt-13191/p-55287</t>
+        </is>
+      </c>
+      <c r="I9" t="inlineStr">
+        <is>
+          <t>polycab_lv_power_cable/images/Polycab_LV_Cu_IEC_60502-1_061kV_MC-3_SWA_image.png</t>
+        </is>
+      </c>
       <c r="J9" t="inlineStr">
         <is>
-          <t>polycab_lv_power_cable/brochures/Polycab_LV_Cu_IEC_60502-1_061kV_MC-4_SWA_datasheet.pdf</t>
+          <t>polycab_lv_power_cable/brochures/Polycab_LV_Cu_IEC_60502-1_061kV_MC-3_SWA_datasheet.pdf</t>
         </is>
       </c>
       <c r="K9" t="inlineStr">
         <is>
-          <t>Not Found</t>
+          <t>Downloaded</t>
         </is>
       </c>
       <c r="L9" t="inlineStr">
@@ -912,7 +1008,7 @@
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>Polycab LV AL IEC 60502-1 0.6/1kV MC-2 SFA</t>
+          <t>Polycab LV IS-7098-I 1C-A2XY</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
@@ -922,35 +1018,47 @@
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>IEC 60502-1, BS 5467</t>
+          <t>IS 7098-I</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>CE, FQC</t>
+          <t>CE, BIS, CPRI, FQC</t>
         </is>
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>UV Resistant, Low Smoke</t>
-        </is>
-      </c>
-      <c r="F10" t="inlineStr"/>
-      <c r="G10" t="inlineStr"/>
+          <t>Higher Current rating, Higher insulation resistance, Better resistance to surge current, Low dielectric losses, Long service life, Higher short circuit rating</t>
+        </is>
+      </c>
+      <c r="F10" t="inlineStr">
+        <is>
+          <t>Single core aluminium, XLPE Insulation, unarmoured ,PVC Outer sheathed cable</t>
+        </is>
+      </c>
+      <c r="G10" t="inlineStr">
+        <is>
+          <t>POLYCAB A2XY SC, stranded compacted aluminium conductor, XLPE insulated, and PVC sheathed confirming to IS 7098-1 is suitable for AC single phase or three phase (earthed or unearthed) systems with rated voltage up to and including 1100 V. This cable is also suitable for DC systems with rated voltage up to and including 1500 V</t>
+        </is>
+      </c>
       <c r="H10" t="inlineStr">
         <is>
-          <t>https://polycab.com/polycab-lv-al-iec-60502-1-061kv-mc-2-sfa/pt-13191/p-55255</t>
-        </is>
-      </c>
-      <c r="I10" t="inlineStr"/>
+          <t>https://polycab.com/polycab-lv-is-7098-i-1c-a2xy/pt-13191/p-54738</t>
+        </is>
+      </c>
+      <c r="I10" t="inlineStr">
+        <is>
+          <t>polycab_lv_power_cable/images/Polycab_LV_IS-7098-I_1C-A2XY_image.png</t>
+        </is>
+      </c>
       <c r="J10" t="inlineStr">
         <is>
-          <t>polycab_lv_power_cable/brochures/Polycab_LV_AL_IEC_60502-1_061kV_MC-2_SFA_datasheet.pdf</t>
+          <t>polycab_lv_power_cable/brochures/Polycab_LV_IS-7098-I_1C-A2XY_datasheet.pdf</t>
         </is>
       </c>
       <c r="K10" t="inlineStr">
         <is>
-          <t>Not Found</t>
+          <t>Downloaded</t>
         </is>
       </c>
       <c r="L10" t="inlineStr">
@@ -972,7 +1080,7 @@
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>IEC 60502-1, BS 5467</t>
+          <t>IEC 60502-1</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
@@ -982,17 +1090,29 @@
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>UV Resistant, Low Smoke</t>
-        </is>
-      </c>
-      <c r="F11" t="inlineStr"/>
-      <c r="G11" t="inlineStr"/>
+          <t>Higher dielectric strength, Better electrical, mechanical, And thermal properties, UV resistant, Long service life, Low smoke emission</t>
+        </is>
+      </c>
+      <c r="F11" t="inlineStr">
+        <is>
+          <t>Single core stranded AL conductor,XLPE/EPR/HEPR insulation, Aluminium strip armoured, PVC/Polyethylene/Halogen free Outer sheathed LV Cable</t>
+        </is>
+      </c>
+      <c r="G11" t="inlineStr">
+        <is>
+          <t>Single core stranded Aluminium conductor, XLPE/EPR/HEPR insulation,PVC/Polyethylene/Halogen free Inner Sheathed, Aluminium strip armored &amp; PVC/Polyethylene/Halogen free Outer sheathed Cable. suitable for fixed installation such as distribution network or industrial installation. These cable cables are designed for systems with rated AC voltage 1KV (Um=1.2 KV).</t>
+        </is>
+      </c>
       <c r="H11" t="inlineStr">
         <is>
           <t>https://polycab.com/polycab-lv-al-iec-60502-1-061kv-sc-sfa/pt-13191/p-55247</t>
         </is>
       </c>
-      <c r="I11" t="inlineStr"/>
+      <c r="I11" t="inlineStr">
+        <is>
+          <t>polycab_lv_power_cable/images/Polycab_LV_AL_IEC_60502-1_061kV_SC_SFA_image.png</t>
+        </is>
+      </c>
       <c r="J11" t="inlineStr">
         <is>
           <t>polycab_lv_power_cable/brochures/Polycab_LV_AL_IEC_60502-1_061kV_SC_SFA_datasheet.pdf</t>
@@ -1000,7 +1120,7 @@
       </c>
       <c r="K11" t="inlineStr">
         <is>
-          <t>Not Found</t>
+          <t>Downloaded</t>
         </is>
       </c>
       <c r="L11" t="inlineStr">
@@ -1012,7 +1132,7 @@
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>Polycab BS 6724 MC SWA LSZH 0.6/1kV AC</t>
+          <t>Polycab LV AL IEC 60502-1 0.6/1kV MC-4 SWA</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
@@ -1022,7 +1142,7 @@
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>IEC 60502-1, BS 6724, BS 5467</t>
+          <t>IEC 60502-1</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
@@ -1032,25 +1152,37 @@
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>High Life, Low Smoke</t>
-        </is>
-      </c>
-      <c r="F12" t="inlineStr"/>
-      <c r="G12" t="inlineStr"/>
+          <t>Higher dielectric strength, Better electrical, mechanical, And thermal properties, UV resistant, Long service life, Low smoke emission</t>
+        </is>
+      </c>
+      <c r="F12" t="inlineStr">
+        <is>
+          <t>Multi core stranded AL conductor, XLPE/EPR/HEPRE insulation, Laid up, Inner covering, Armoured, PVC/Polyethylene/Halogen free Outer sheathed LV Cable</t>
+        </is>
+      </c>
+      <c r="G12" t="inlineStr">
+        <is>
+          <t>Multicore stranded Aluminium, XLPE/EPR/HEPR insulation, Laid up, inner covering,GI wire,PVC/Polyethylene/Halogen free sheathed Cable suitable for fixed installation such as distribution network or industrial installation.These cables are designed for systems with rated AC voltage 1KV (Um=1.2 KV) between two live conductor.</t>
+        </is>
+      </c>
       <c r="H12" t="inlineStr">
         <is>
-          <t>https://polycab.com/polycab-bs-6724-mc-swa-lszh-061kv-ac/pt-13191/p-55457</t>
-        </is>
-      </c>
-      <c r="I12" t="inlineStr"/>
+          <t>https://polycab.com/polycab-lv-al-iec-60502-1-061kv-mc-4-swa/pt-13191/p-55293</t>
+        </is>
+      </c>
+      <c r="I12" t="inlineStr">
+        <is>
+          <t>polycab_lv_power_cable/images/Polycab_LV_AL_IEC_60502-1_061kV_MC-4_SWA_image.png</t>
+        </is>
+      </c>
       <c r="J12" t="inlineStr">
         <is>
-          <t>polycab_lv_power_cable/brochures/Polycab_BS_6724_MC_SWA_LSZH_061kV_AC_datasheet.pdf</t>
+          <t>polycab_lv_power_cable/brochures/Polycab_LV_AL_IEC_60502-1_061kV_MC-4_SWA_datasheet.pdf</t>
         </is>
       </c>
       <c r="K12" t="inlineStr">
         <is>
-          <t>Not Found</t>
+          <t>Downloaded</t>
         </is>
       </c>
       <c r="L12" t="inlineStr">
@@ -1062,7 +1194,7 @@
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>Polycab LV AL IEC 60502-1 0.6/1kV MC-3.5 UA</t>
+          <t>Polycab LV AL IEC 60502-1 0.6/1kV MC-2 SFA</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
@@ -1072,7 +1204,7 @@
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>IEC 60502-1, BS 5467</t>
+          <t>IEC 60502-1</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
@@ -1082,25 +1214,37 @@
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>UV Resistant, Low Smoke</t>
-        </is>
-      </c>
-      <c r="F13" t="inlineStr"/>
-      <c r="G13" t="inlineStr"/>
+          <t>Higher dielectric strength, Better electrical, mechanical, And thermal properties, UV resistant, Long service life, Low smoke emission</t>
+        </is>
+      </c>
+      <c r="F13" t="inlineStr">
+        <is>
+          <t>Multi core stranded AL conductor, XLPE/EPR/HEPR insulation, Laid up, Inner covering, Armoured, PVC/Polyethylene/Halogen free Outer sheathed LV Cablee</t>
+        </is>
+      </c>
+      <c r="G13" t="inlineStr">
+        <is>
+          <t>Multicore stranded Aluminium, XLPE/EPR/HEPR insulation, Laid up, inner covering,GI flat strip,PVC/Polyethylene/Halogen free sheathed Cable suitable for fixed installation such as distribution network or industrial installation.These cables are designed for systems with rated AC voltage 1KV (Um=1.2 KV) between two live conductor.</t>
+        </is>
+      </c>
       <c r="H13" t="inlineStr">
         <is>
-          <t>https://polycab.com/polycab-lv-al-iec-60502-1-061kv-mc-35-ua/pt-13191/p-55271</t>
-        </is>
-      </c>
-      <c r="I13" t="inlineStr"/>
+          <t>https://polycab.com/polycab-lv-al-iec-60502-1-061kv-mc-2-sfa/pt-13191/p-55255</t>
+        </is>
+      </c>
+      <c r="I13" t="inlineStr">
+        <is>
+          <t>polycab_lv_power_cable/images/Polycab_LV_AL_IEC_60502-1_061kV_MC-2_SFA_image.png</t>
+        </is>
+      </c>
       <c r="J13" t="inlineStr">
         <is>
-          <t>polycab_lv_power_cable/brochures/Polycab_LV_AL_IEC_60502-1_061kV_MC-35_UA_datasheet.pdf</t>
+          <t>polycab_lv_power_cable/brochures/Polycab_LV_AL_IEC_60502-1_061kV_MC-2_SFA_datasheet.pdf</t>
         </is>
       </c>
       <c r="K13" t="inlineStr">
         <is>
-          <t>Not Found</t>
+          <t>Downloaded</t>
         </is>
       </c>
       <c r="L13" t="inlineStr">
@@ -1112,7 +1256,7 @@
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>Polycab LV IS-7098-I 3.5C A2XFY</t>
+          <t>Polycab LV AL IEC 60502-1 0.6/1kV SC UA</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
@@ -1122,31 +1266,47 @@
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>IEC 60502-1, IS 7098-1, BS 5467</t>
+          <t>IEC 60502-1</t>
         </is>
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>CE, BIS, CPRI, FQC</t>
-        </is>
-      </c>
-      <c r="E14" t="inlineStr"/>
-      <c r="F14" t="inlineStr"/>
-      <c r="G14" t="inlineStr"/>
+          <t>CE, FQC</t>
+        </is>
+      </c>
+      <c r="E14" t="inlineStr">
+        <is>
+          <t>Higher dielectric strength, Better electrical, mechanical, And thermal properties, UV resistant, Long service life, Low smoke emission</t>
+        </is>
+      </c>
+      <c r="F14" t="inlineStr">
+        <is>
+          <t>Single core stranded AL conductor,XLPE/EPR/HEPR insulation, unarmoured,PVC/Polyethylene/Halogen free Outer sheathed LV Cable</t>
+        </is>
+      </c>
+      <c r="G14" t="inlineStr">
+        <is>
+          <t>Single core stranded Aluminium conductor, XLPE/EPR/HEPR insulation,PVC/Polyethylene/Halogen free Inner &amp; outer sheathed Cable. suitable for fixed installation such as distribution network or industrial installation. These cable cables are designed for systems with rated AC voltage 1KV (Um=1.2 KV).</t>
+        </is>
+      </c>
       <c r="H14" t="inlineStr">
         <is>
-          <t>https://polycab.com/polycab-lv-is-7098-i-35c-a2xfy/pt-13191/p-54712</t>
-        </is>
-      </c>
-      <c r="I14" t="inlineStr"/>
+          <t>https://polycab.com/polycab-lv-al-iec-60502-1-061kv-sc-ua/pt-13191/p-55243</t>
+        </is>
+      </c>
+      <c r="I14" t="inlineStr">
+        <is>
+          <t>polycab_lv_power_cable/images/Polycab_LV_AL_IEC_60502-1_061kV_SC_UA_image.png</t>
+        </is>
+      </c>
       <c r="J14" t="inlineStr">
         <is>
-          <t>polycab_lv_power_cable/brochures/Polycab_LV_IS-7098-I_35C_A2XFY_datasheet.pdf</t>
+          <t>polycab_lv_power_cable/brochures/Polycab_LV_AL_IEC_60502-1_061kV_SC_UA_datasheet.pdf</t>
         </is>
       </c>
       <c r="K14" t="inlineStr">
         <is>
-          <t>Not Found</t>
+          <t>Downloaded</t>
         </is>
       </c>
       <c r="L14" t="inlineStr">
@@ -1158,7 +1318,7 @@
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>Polycab LV Cu IEC 60502-1 0.6/1kV MC-4 UA</t>
+          <t>Polycab LV AL IEC 60502-1 0.6/1kV SC AWA</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
@@ -1168,7 +1328,7 @@
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>IEC 60502-1, BS 5467</t>
+          <t>IEC 60502-1</t>
         </is>
       </c>
       <c r="D15" t="inlineStr">
@@ -1178,25 +1338,37 @@
       </c>
       <c r="E15" t="inlineStr">
         <is>
-          <t>UV Resistant, Low Smoke</t>
-        </is>
-      </c>
-      <c r="F15" t="inlineStr"/>
-      <c r="G15" t="inlineStr"/>
+          <t>Higher dielectric strength, Better electrical, mechanical, And thermal properties, UV resistant, Long service life, Low smoke emission</t>
+        </is>
+      </c>
+      <c r="F15" t="inlineStr">
+        <is>
+          <t>Single core stranded AL conductor,XLPE/EPR/HEPR insulation,Aluminium armoured,PVC/Polyethylene/Halogen free Outer sheathed LV Cable</t>
+        </is>
+      </c>
+      <c r="G15" t="inlineStr">
+        <is>
+          <t>Single core stranded Aluminium conductor, XLPE/EPR/HEPR insulation,PVC/Polyethylene/Halogen free Inner, Aluminium wire armored &amp; outer sheathed Cable. suitable for fixed installation such as distribution network or industrial installation. These cable cables are designed for systems with rated AC voltage 1KV (Um=1.2 KV).</t>
+        </is>
+      </c>
       <c r="H15" t="inlineStr">
         <is>
-          <t>https://polycab.com/polycab-lv-cu-iec-60502-1-061kv-mc-4-ua/pt-13191/p-55301</t>
-        </is>
-      </c>
-      <c r="I15" t="inlineStr"/>
+          <t>https://polycab.com/polycab-lv-al-iec-60502-1-061kv-sc-awa/pt-13191/p-55245</t>
+        </is>
+      </c>
+      <c r="I15" t="inlineStr">
+        <is>
+          <t>polycab_lv_power_cable/images/Polycab_LV_AL_IEC_60502-1_061kV_SC_AWA_image.png</t>
+        </is>
+      </c>
       <c r="J15" t="inlineStr">
         <is>
-          <t>polycab_lv_power_cable/brochures/Polycab_LV_Cu_IEC_60502-1_061kV_MC-4_UA_datasheet.pdf</t>
+          <t>polycab_lv_power_cable/brochures/Polycab_LV_AL_IEC_60502-1_061kV_SC_AWA_datasheet.pdf</t>
         </is>
       </c>
       <c r="K15" t="inlineStr">
         <is>
-          <t>Not Found</t>
+          <t>Downloaded</t>
         </is>
       </c>
       <c r="L15" t="inlineStr">
@@ -1208,7 +1380,7 @@
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>Polycab LV Cu IEC 60502-1 0.6/1kV MC-3.5 SWA</t>
+          <t>Polycab LV AL IEC 60502-1 0.6/1kV MC-3 SFA</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
@@ -1218,7 +1390,7 @@
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>IEC 60502-1, BS 5467</t>
+          <t>IEC 60502-1</t>
         </is>
       </c>
       <c r="D16" t="inlineStr">
@@ -1228,25 +1400,37 @@
       </c>
       <c r="E16" t="inlineStr">
         <is>
-          <t>UV Resistant, Low Smoke</t>
-        </is>
-      </c>
-      <c r="F16" t="inlineStr"/>
-      <c r="G16" t="inlineStr"/>
+          <t>Higher dielectric strength, Better electrical, mechanical, And thermal properties, UV resistant, Long service life, Low smoke emission</t>
+        </is>
+      </c>
+      <c r="F16" t="inlineStr">
+        <is>
+          <t>Multi core stranded AL conductor, XLPE/EPR/HEPR insulation, Laid up, Inner covering, Armoured,PVC/Polyethylene/Halogen free inner &amp; Outer sheathed LV Cable</t>
+        </is>
+      </c>
+      <c r="G16" t="inlineStr">
+        <is>
+          <t>Multicore stranded Aluminium conductor, XLPE/EPR/HEPR insulation, Laid up, inner covering,GI flat strip armoured,PVC/Polyethylene/Halogen free sheathed. suitable for fixed installation such as distribution network or industrial installation. These cable cables are designed for systems with rated AC voltage 1KV (Um=1.2 KV) between two live conductor.</t>
+        </is>
+      </c>
       <c r="H16" t="inlineStr">
         <is>
-          <t>https://polycab.com/polycab-lv-cu-iec-60502-1-061kv-mc-35-swa/pt-13191/p-55275</t>
-        </is>
-      </c>
-      <c r="I16" t="inlineStr"/>
+          <t>https://polycab.com/polycab-lv-al-iec-60502-1-061kv-mc-3-sfa/pt-13191/p-55279</t>
+        </is>
+      </c>
+      <c r="I16" t="inlineStr">
+        <is>
+          <t>polycab_lv_power_cable/images/Polycab_LV_AL_IEC_60502-1_061kV_MC-3_SFA_image.png</t>
+        </is>
+      </c>
       <c r="J16" t="inlineStr">
         <is>
-          <t>polycab_lv_power_cable/brochures/Polycab_LV_Cu_IEC_60502-1_061kV_MC-35_SWA_datasheet.pdf</t>
+          <t>polycab_lv_power_cable/brochures/Polycab_LV_AL_IEC_60502-1_061kV_MC-3_SFA_datasheet.pdf</t>
         </is>
       </c>
       <c r="K16" t="inlineStr">
         <is>
-          <t>Not Found</t>
+          <t>Downloaded</t>
         </is>
       </c>
       <c r="L16" t="inlineStr">
@@ -1258,7 +1442,7 @@
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>Polycab LV IS-7098-I 3C-2XY</t>
+          <t>Polycab LV Cu IEC 60502-1 0.6/1kV MC-3.5 SFA</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
@@ -1268,31 +1452,47 @@
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>IEC 60502-1, IS 7098-1, BS 5467</t>
+          <t>IEC 60502-1</t>
         </is>
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>CE, BIS, CPRI, FQC</t>
-        </is>
-      </c>
-      <c r="E17" t="inlineStr"/>
-      <c r="F17" t="inlineStr"/>
-      <c r="G17" t="inlineStr"/>
+          <t>CE, FQC</t>
+        </is>
+      </c>
+      <c r="E17" t="inlineStr">
+        <is>
+          <t>Higher dielectric strength, Better electrical, mechanical, And thermal properties, UV resistant, Long service life, Low smoke emission</t>
+        </is>
+      </c>
+      <c r="F17" t="inlineStr">
+        <is>
+          <t>Multi core stranded copper conductor,XLPE/EPR/HEPR insulation, Laid up, Inner covering, Armoured, PVC/Polyethylene/Halogen free Outer sheathed LV Cable</t>
+        </is>
+      </c>
+      <c r="G17" t="inlineStr">
+        <is>
+          <t>Multicore stranded Copper conductor, XLPE/EPR/HEPR insulation, Laid up, inner covering,GI flat strip armoured,PVC/Polyethylene/Halogen free sheathed. suitable for fixed installation such as distribution network or industrial installation. These cable cables are designed for systems with rated AC voltage 1KV (Um=1.2 KV) between two live conductor.</t>
+        </is>
+      </c>
       <c r="H17" t="inlineStr">
         <is>
-          <t>https://polycab.com/polycab-lv-is-7098-i-3c-2xy/pt-13191/p-54748</t>
-        </is>
-      </c>
-      <c r="I17" t="inlineStr"/>
+          <t>https://polycab.com/polycab-lv-cu-iec-60502-1-061kv-mc-35-sfa/pt-13191/p-55273</t>
+        </is>
+      </c>
+      <c r="I17" t="inlineStr">
+        <is>
+          <t>polycab_lv_power_cable/images/Polycab_LV_Cu_IEC_60502-1_061kV_MC-35_SFA_image.png</t>
+        </is>
+      </c>
       <c r="J17" t="inlineStr">
         <is>
-          <t>polycab_lv_power_cable/brochures/Polycab_LV_IS-7098-I_3C-2XY_datasheet.pdf</t>
+          <t>polycab_lv_power_cable/brochures/Polycab_LV_Cu_IEC_60502-1_061kV_MC-35_SFA_datasheet.pdf</t>
         </is>
       </c>
       <c r="K17" t="inlineStr">
         <is>
-          <t>Not Found</t>
+          <t>Downloaded</t>
         </is>
       </c>
       <c r="L17" t="inlineStr">
@@ -1304,7 +1504,7 @@
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>Polycab LV AL IEC 60502-1 0.6/1kV MC-3.5 SWA</t>
+          <t>Polycab LV Cu IEC 60502-1 0.6/1kV MC-3.5 SWA</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
@@ -1314,7 +1514,7 @@
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>IEC 60502-1, BS 5467</t>
+          <t>IEC 60502-1</t>
         </is>
       </c>
       <c r="D18" t="inlineStr">
@@ -1324,25 +1524,37 @@
       </c>
       <c r="E18" t="inlineStr">
         <is>
-          <t>UV Resistant, Low Smoke</t>
-        </is>
-      </c>
-      <c r="F18" t="inlineStr"/>
-      <c r="G18" t="inlineStr"/>
+          <t>Higher dielectric strength, Better electrical, mechanical, And thermal properties, UV resistant, Long service life, Low smoke emission</t>
+        </is>
+      </c>
+      <c r="F18" t="inlineStr">
+        <is>
+          <t>Multi core stranded copper conductor,XLPE/EPR/HEPR insulation, Laid up, Inner covering, Armoured, PVC/Polyethylene/Halogen free Outer sheathed LV Cable</t>
+        </is>
+      </c>
+      <c r="G18" t="inlineStr">
+        <is>
+          <t>Multicore stranded Copper, XLPE/EPR/HEPR insulation, Laid up, inner covering,GI wire,PVC/Polyethylene/Halogen free sheathed Cable suitable for fixed installation such as distribution network or industrial installation.These cables are designed for systems with rated AC voltage 1KV (Um=1.2 KV) between two live conductor.</t>
+        </is>
+      </c>
       <c r="H18" t="inlineStr">
         <is>
-          <t>https://polycab.com/polycab-lv-al-iec-60502-1-061kv-mc-35-swa/pt-13191/p-55269</t>
-        </is>
-      </c>
-      <c r="I18" t="inlineStr"/>
+          <t>https://polycab.com/polycab-lv-cu-iec-60502-1-061kv-mc-35-swa/pt-13191/p-55275</t>
+        </is>
+      </c>
+      <c r="I18" t="inlineStr">
+        <is>
+          <t>polycab_lv_power_cable/images/Polycab_LV_Cu_IEC_60502-1_061kV_MC-35_SWA_image.png</t>
+        </is>
+      </c>
       <c r="J18" t="inlineStr">
         <is>
-          <t>polycab_lv_power_cable/brochures/Polycab_LV_AL_IEC_60502-1_061kV_MC-35_SWA_datasheet.pdf</t>
+          <t>polycab_lv_power_cable/brochures/Polycab_LV_Cu_IEC_60502-1_061kV_MC-35_SWA_datasheet.pdf</t>
         </is>
       </c>
       <c r="K18" t="inlineStr">
         <is>
-          <t>Not Found</t>
+          <t>Downloaded</t>
         </is>
       </c>
       <c r="L18" t="inlineStr">
@@ -1354,7 +1566,7 @@
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>Polycab LV IS-7098-I 4C 2XWY</t>
+          <t>Polycab LV AL IEC 60502-1 0.6/1kV MC-4 SFA</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
@@ -1364,31 +1576,47 @@
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>IEC 60502-1, IS 7098-1, BS 5467</t>
+          <t>IEC 60502-1</t>
         </is>
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>CE, BIS, CPRI, FQC</t>
-        </is>
-      </c>
-      <c r="E19" t="inlineStr"/>
-      <c r="F19" t="inlineStr"/>
-      <c r="G19" t="inlineStr"/>
+          <t>CE, FQC</t>
+        </is>
+      </c>
+      <c r="E19" t="inlineStr">
+        <is>
+          <t>Higher dielectric strength, Better electrical, mechanical, And thermal properties, UV resistant, Long service life, Low smoke emission</t>
+        </is>
+      </c>
+      <c r="F19" t="inlineStr">
+        <is>
+          <t>Multi core stranded AL conductor,XLPE/EPR/HEPR insulation, Laid up, Inner covering, Armoured,PVC/Polyethylene/Halogen free Outer sheathed LV Cable</t>
+        </is>
+      </c>
+      <c r="G19" t="inlineStr">
+        <is>
+          <t>Multicore stranded Aluminium conductor, XLPE/EPR/HEPR insulation, Laid up, inner covering,GI flat strip armoured,PVC/Polyethylene/Halogen free sheathed. suitable for fixed installation such as distribution network or industrial installation. These cable cables are designed for systems with rated AC voltage 1KV (Um=1.2 KV) between two live conductor.</t>
+        </is>
+      </c>
       <c r="H19" t="inlineStr">
         <is>
-          <t>https://polycab.com/polycab-lv-is-7098-i-4c-2xwy/pt-13191/p-54726</t>
-        </is>
-      </c>
-      <c r="I19" t="inlineStr"/>
+          <t>https://polycab.com/polycab-lv-al-iec-60502-1-061kv-mc-4-sfa/pt-13191/p-55291</t>
+        </is>
+      </c>
+      <c r="I19" t="inlineStr">
+        <is>
+          <t>polycab_lv_power_cable/images/Polycab_LV_AL_IEC_60502-1_061kV_MC-4_SFA_image.png</t>
+        </is>
+      </c>
       <c r="J19" t="inlineStr">
         <is>
-          <t>polycab_lv_power_cable/brochures/Polycab_LV_IS-7098-I_4C_2XWY_datasheet.pdf</t>
+          <t>polycab_lv_power_cable/brochures/Polycab_LV_AL_IEC_60502-1_061kV_MC-4_SFA_datasheet.pdf</t>
         </is>
       </c>
       <c r="K19" t="inlineStr">
         <is>
-          <t>Not Found</t>
+          <t>Downloaded</t>
         </is>
       </c>
       <c r="L19" t="inlineStr">
@@ -1400,7 +1628,7 @@
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>Polycab LV AL IEC 60502-1 0.6/1kV MC-3.5 SFA</t>
+          <t>Polycab LV IS-7098-I 4C 2XFY</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
@@ -1410,35 +1638,47 @@
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>IEC 60502-1, BS 5467</t>
+          <t>IS 7098-I</t>
         </is>
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>CE, FQC</t>
+          <t>CE, BIS, CPRI, FQC</t>
         </is>
       </c>
       <c r="E20" t="inlineStr">
         <is>
-          <t>UV Resistant, Low Smoke</t>
-        </is>
-      </c>
-      <c r="F20" t="inlineStr"/>
-      <c r="G20" t="inlineStr"/>
+          <t>Higher Current rating, Higher insulation resistance, Better resistance to surge current, Low dielectric losses, Long service life, Higher short circuit rating</t>
+        </is>
+      </c>
+      <c r="F20" t="inlineStr">
+        <is>
+          <t>Four core copper, XLPE Insulation, Inner sheathed &amp; GI flat armoured &amp; PVC Outer sheathed cable</t>
+        </is>
+      </c>
+      <c r="G20" t="inlineStr">
+        <is>
+          <t>POLYCAB 2XFY MC-4,Stranded compacted copper conductor, XLPE insulated, PVC inner sheathed, Galvanised Steel Flat strip armour and PVC sheathed confirming to IS 7098-1 is suitable for AC single phase or three phase (earthed or unearthed) systems with rated voltage up to and including 1100 V. This cable is also suitable for DC systems with rated voltage up to and including 1500 V</t>
+        </is>
+      </c>
       <c r="H20" t="inlineStr">
         <is>
-          <t>https://polycab.com/polycab-lv-al-iec-60502-1-061kv-mc-35-sfa/pt-13191/p-55267</t>
-        </is>
-      </c>
-      <c r="I20" t="inlineStr"/>
+          <t>https://polycab.com/polycab-lv-is-7098-i-4c-2xfy/pt-13191/p-54724</t>
+        </is>
+      </c>
+      <c r="I20" t="inlineStr">
+        <is>
+          <t>polycab_lv_power_cable/images/Polycab_LV_IS-7098-I_4C_2XFY_image.png</t>
+        </is>
+      </c>
       <c r="J20" t="inlineStr">
         <is>
-          <t>polycab_lv_power_cable/brochures/Polycab_LV_AL_IEC_60502-1_061kV_MC-35_SFA_datasheet.pdf</t>
+          <t>polycab_lv_power_cable/brochures/Polycab_LV_IS-7098-I_4C_2XFY_datasheet.pdf</t>
         </is>
       </c>
       <c r="K20" t="inlineStr">
         <is>
-          <t>Not Found</t>
+          <t>Downloaded</t>
         </is>
       </c>
       <c r="L20" t="inlineStr">
@@ -1450,7 +1690,7 @@
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>Polycab LV Cu IEC 60502-1 0.6/1kV MC-3 UA</t>
+          <t>Polycab LV AL IEC 60502-1 0.6/1kV MC-3.5 SFA</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
@@ -1460,7 +1700,7 @@
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>IEC 60502-1, BS 5467</t>
+          <t>IEC 60502-1</t>
         </is>
       </c>
       <c r="D21" t="inlineStr">
@@ -1470,25 +1710,37 @@
       </c>
       <c r="E21" t="inlineStr">
         <is>
-          <t>UV Resistant, Low Smoke</t>
-        </is>
-      </c>
-      <c r="F21" t="inlineStr"/>
-      <c r="G21" t="inlineStr"/>
+          <t>Higher dielectric strength, Better electrical, mechanical, And thermal properties, UV resistant, Long service life, Low smoke emission</t>
+        </is>
+      </c>
+      <c r="F21" t="inlineStr">
+        <is>
+          <t>Multi core stranded AL conductor, XLPE/EPR/HEPR insulation, Laid up, Inner covering, Armoured, PVC/Polyethylene/Halogen free Outer sheathed LV Cable</t>
+        </is>
+      </c>
+      <c r="G21" t="inlineStr">
+        <is>
+          <t>Multicore stranded Aluminium conductor, XLPE/EPR/HEPR insulation, Laid up, inner covering,GI flat strip armoured,PVC/Polyethylene/Halogen free sheathed. suitable for fixed installation such as distribution network or industrial installation. These cable cables are designed for systems with rated AC voltage 1KV (Um=1.2 KV) between two live conductor.</t>
+        </is>
+      </c>
       <c r="H21" t="inlineStr">
         <is>
-          <t>https://polycab.com/polycab-lv-cu-iec-60502-1-061kv-mc-3-ua/pt-13191/p-55289</t>
-        </is>
-      </c>
-      <c r="I21" t="inlineStr"/>
+          <t>https://polycab.com/polycab-lv-al-iec-60502-1-061kv-mc-35-sfa/pt-13191/p-55267</t>
+        </is>
+      </c>
+      <c r="I21" t="inlineStr">
+        <is>
+          <t>polycab_lv_power_cable/images/Polycab_LV_AL_IEC_60502-1_061kV_MC-35_SFA_image.png</t>
+        </is>
+      </c>
       <c r="J21" t="inlineStr">
         <is>
-          <t>polycab_lv_power_cable/brochures/Polycab_LV_Cu_IEC_60502-1_061kV_MC-3_UA_datasheet.pdf</t>
+          <t>polycab_lv_power_cable/brochures/Polycab_LV_AL_IEC_60502-1_061kV_MC-35_SFA_datasheet.pdf</t>
         </is>
       </c>
       <c r="K21" t="inlineStr">
         <is>
-          <t>Not Found</t>
+          <t>Downloaded</t>
         </is>
       </c>
       <c r="L21" t="inlineStr">
@@ -1500,7 +1752,7 @@
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>Polycab LV IS-7098-I 1C-A2XY</t>
+          <t>Polycab LV Cu IEC 60502-1 0.6/1kV SC SFA</t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
@@ -1510,31 +1762,47 @@
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>IEC 60502-1, IS 7098-1, BS 5467</t>
+          <t>IEC 60502-1</t>
         </is>
       </c>
       <c r="D22" t="inlineStr">
         <is>
-          <t>CE, BIS, CPRI, FQC</t>
-        </is>
-      </c>
-      <c r="E22" t="inlineStr"/>
-      <c r="F22" t="inlineStr"/>
-      <c r="G22" t="inlineStr"/>
+          <t>CE, FQC</t>
+        </is>
+      </c>
+      <c r="E22" t="inlineStr">
+        <is>
+          <t>Higher dielectric strength, Better electrical, mechanical, And thermal properties, UV resistant, Long service life, Low smoke emission</t>
+        </is>
+      </c>
+      <c r="F22" t="inlineStr">
+        <is>
+          <t>Single core stranded Copper conductor,XLPE/EPR/HEPR insulation, Aluminium strip armoured unarmoured, PVC/Polyethylene/Halogen free Outer sheathed LV Cable</t>
+        </is>
+      </c>
+      <c r="G22" t="inlineStr">
+        <is>
+          <t>Single core stranded Copper conductor, XLPE/EPR/HEPR insulation,PVC/Polyethylene/Halogen free Inner Sheathed, Aluminium strip armored &amp; PVC/Polyethylene/Halogen free Outer sheathed Cable. suitable for fixed installation such as distribution network or industrial installation. These cable cables are designed for systems with rated AC voltage 1KV (Um=1.2 KV).</t>
+        </is>
+      </c>
       <c r="H22" t="inlineStr">
         <is>
-          <t>https://polycab.com/polycab-lv-is-7098-i-1c-a2xy/pt-13191/p-54738</t>
-        </is>
-      </c>
-      <c r="I22" t="inlineStr"/>
+          <t>https://polycab.com/polycab-lv-cu-iec-60502-1-061kv-sc-sfa/pt-13191/p-55251</t>
+        </is>
+      </c>
+      <c r="I22" t="inlineStr">
+        <is>
+          <t>polycab_lv_power_cable/images/Polycab_LV_Cu_IEC_60502-1_061kV_SC_SFA_image.png</t>
+        </is>
+      </c>
       <c r="J22" t="inlineStr">
         <is>
-          <t>polycab_lv_power_cable/brochures/Polycab_LV_IS-7098-I_1C-A2XY_datasheet.pdf</t>
+          <t>polycab_lv_power_cable/brochures/Polycab_LV_Cu_IEC_60502-1_061kV_SC_SFA_datasheet.pdf</t>
         </is>
       </c>
       <c r="K22" t="inlineStr">
         <is>
-          <t>Not Found</t>
+          <t>Downloaded</t>
         </is>
       </c>
       <c r="L22" t="inlineStr">
@@ -1546,7 +1814,7 @@
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>Polycab LV AL IEC 60502-1 0.6/1kV MC-3 SWA</t>
+          <t>Polycab LV IS-7098-I 3.5C 2XWY</t>
         </is>
       </c>
       <c r="B23" t="inlineStr">
@@ -1556,35 +1824,47 @@
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>IEC 60502-1, BS 5467</t>
+          <t>IS 7098-I</t>
         </is>
       </c>
       <c r="D23" t="inlineStr">
         <is>
-          <t>CE, FQC</t>
+          <t>CE, BIS, CPRI, FQC</t>
         </is>
       </c>
       <c r="E23" t="inlineStr">
         <is>
-          <t>UV Resistant, Low Smoke</t>
-        </is>
-      </c>
-      <c r="F23" t="inlineStr"/>
-      <c r="G23" t="inlineStr"/>
+          <t>Higher Current rating, Higher insulation resistance, Better resistance to surge current, Low dielectric losses, Long service life, Higher short circuit rating</t>
+        </is>
+      </c>
+      <c r="F23" t="inlineStr">
+        <is>
+          <t>Three and half core Copper conductor, XLPE Insulation Inner sheathed &amp; GI round armoured &amp; PVC Outer sheathed cable</t>
+        </is>
+      </c>
+      <c r="G23" t="inlineStr">
+        <is>
+          <t>POLYCAB 2XWY MC-3.5, Stranded compacted copper conductor ,XLPE insulated, PVC inner sheathed, Galvanised Steel round wire armour and PVC sheathed confirming to IS 7098-1 is suitable for AC single phase or three phase (earthed or unearthed) systems with rated voltage up to and including 1100 V. This cable is also suitable for DC systems with rated voltage up to and including 1500 V</t>
+        </is>
+      </c>
       <c r="H23" t="inlineStr">
         <is>
-          <t>https://polycab.com/polycab-lv-al-iec-60502-1-061kv-mc-3-swa/pt-13191/p-55281</t>
-        </is>
-      </c>
-      <c r="I23" t="inlineStr"/>
+          <t>https://polycab.com/polycab-lv-is-7098-i-35c-2xwy/pt-13191/p-54710</t>
+        </is>
+      </c>
+      <c r="I23" t="inlineStr">
+        <is>
+          <t>polycab_lv_power_cable/images/Polycab_LV_IS-7098-I_35C_2XWY_image.png</t>
+        </is>
+      </c>
       <c r="J23" t="inlineStr">
         <is>
-          <t>polycab_lv_power_cable/brochures/Polycab_LV_AL_IEC_60502-1_061kV_MC-3_SWA_datasheet.pdf</t>
+          <t>polycab_lv_power_cable/brochures/Polycab_LV_IS-7098-I_35C_2XWY_datasheet.pdf</t>
         </is>
       </c>
       <c r="K23" t="inlineStr">
         <is>
-          <t>Not Found</t>
+          <t>Downloaded</t>
         </is>
       </c>
       <c r="L23" t="inlineStr">
@@ -1596,7 +1876,7 @@
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>Polycab LV IS-7098-I 2C 2XWY</t>
+          <t>Polycab LV AL IEC 60502-1 0.6/1kV MC-4 UA</t>
         </is>
       </c>
       <c r="B24" t="inlineStr">
@@ -1606,31 +1886,47 @@
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>IEC 60502-1, IS 7098-1, BS 5467</t>
+          <t>IEC 60502-1</t>
         </is>
       </c>
       <c r="D24" t="inlineStr">
         <is>
-          <t>CE, BIS, CPRI, FQC</t>
-        </is>
-      </c>
-      <c r="E24" t="inlineStr"/>
-      <c r="F24" t="inlineStr"/>
-      <c r="G24" t="inlineStr"/>
+          <t>CE, FQC</t>
+        </is>
+      </c>
+      <c r="E24" t="inlineStr">
+        <is>
+          <t>Higher dielectric strength, Better electrical, mechanical, And thermal properties, UV resistant, Long service life, Low smoke emission</t>
+        </is>
+      </c>
+      <c r="F24" t="inlineStr">
+        <is>
+          <t>Multi core stranded AL conductor, XLPE/EPR/HEPR insulation, Laid up, Inner covering, Armoured, PVC/Polyethylene/Halogen free Outer sheathed LV Cable</t>
+        </is>
+      </c>
+      <c r="G24" t="inlineStr">
+        <is>
+          <t>Multicore stranded Aluminium, XLPE/EPR/HEPR insulation, Laid up, inner covering,PVC/Polyethylene/Halogen free sheathed unarmored Cable suitable for fixed installation such as distribution network or industrial installation.These cables are designed for systems with rated AC voltage 1KV (Um=1.2 KV) between two live conductor.</t>
+        </is>
+      </c>
       <c r="H24" t="inlineStr">
         <is>
-          <t>https://polycab.com/polycab-lv-is-7098-i-2c-2xwy/pt-13191/p-54702</t>
-        </is>
-      </c>
-      <c r="I24" t="inlineStr"/>
+          <t>https://polycab.com/polycab-lv-al-iec-60502-1-061kv-mc-4-ua/pt-13191/p-55295</t>
+        </is>
+      </c>
+      <c r="I24" t="inlineStr">
+        <is>
+          <t>polycab_lv_power_cable/images/Polycab_LV_AL_IEC_60502-1_061kV_MC-4_UA_image.png</t>
+        </is>
+      </c>
       <c r="J24" t="inlineStr">
         <is>
-          <t>polycab_lv_power_cable/brochures/Polycab_LV_IS-7098-I_2C_2XWY_datasheet.pdf</t>
+          <t>polycab_lv_power_cable/brochures/Polycab_LV_AL_IEC_60502-1_061kV_MC-4_UA_datasheet.pdf</t>
         </is>
       </c>
       <c r="K24" t="inlineStr">
         <is>
-          <t>Not Found</t>
+          <t>Downloaded</t>
         </is>
       </c>
       <c r="L24" t="inlineStr">
@@ -1642,7 +1938,7 @@
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>Polycab LV IS-7098-I 2C 2XFY</t>
+          <t>Polycab LV AL IEC 60502-1 0.6/1kV MC-3.5 SWA</t>
         </is>
       </c>
       <c r="B25" t="inlineStr">
@@ -1652,31 +1948,47 @@
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>IEC 60502-1, IS 7098-1, BS 5467</t>
+          <t>IEC 60502-1</t>
         </is>
       </c>
       <c r="D25" t="inlineStr">
         <is>
-          <t>CE, BIS, CPRI, FQC</t>
-        </is>
-      </c>
-      <c r="E25" t="inlineStr"/>
-      <c r="F25" t="inlineStr"/>
-      <c r="G25" t="inlineStr"/>
+          <t>CE, FQC</t>
+        </is>
+      </c>
+      <c r="E25" t="inlineStr">
+        <is>
+          <t>Higher dielectric strength, Better electrical, mechanical, And thermal properties, UV resistant, Long service life, Low smoke emission</t>
+        </is>
+      </c>
+      <c r="F25" t="inlineStr">
+        <is>
+          <t>Multi core stranded AL conductor, XLPE/EPR/HEPR insulation, Laid up, Inner covering, Armoured, PVC/Polyethylene/Halogen free Outer sheathed LV Cable</t>
+        </is>
+      </c>
+      <c r="G25" t="inlineStr">
+        <is>
+          <t>Multicore stranded Aluminium, XLPE/EPR/HEPR insulation, Laid up, inner covering,GI wire,PVC/Polyethylene/Halogen free sheathed Cable suitable for fixed installation such as distribution network or industrial installation.These cables are designed for systems with rated AC voltage 1KV (Um=1.2 KV) between two live conductor.</t>
+        </is>
+      </c>
       <c r="H25" t="inlineStr">
         <is>
-          <t>https://polycab.com/polycab-lv-is-7098-i-2c-2xfy/pt-13191/p-54700</t>
-        </is>
-      </c>
-      <c r="I25" t="inlineStr"/>
+          <t>https://polycab.com/polycab-lv-al-iec-60502-1-061kv-mc-35-swa/pt-13191/p-55269</t>
+        </is>
+      </c>
+      <c r="I25" t="inlineStr">
+        <is>
+          <t>polycab_lv_power_cable/images/Polycab_LV_AL_IEC_60502-1_061kV_MC-35_SWA_image.png</t>
+        </is>
+      </c>
       <c r="J25" t="inlineStr">
         <is>
-          <t>polycab_lv_power_cable/brochures/Polycab_LV_IS-7098-I_2C_2XFY_datasheet.pdf</t>
+          <t>polycab_lv_power_cable/brochures/Polycab_LV_AL_IEC_60502-1_061kV_MC-35_SWA_datasheet.pdf</t>
         </is>
       </c>
       <c r="K25" t="inlineStr">
         <is>
-          <t>Not Found</t>
+          <t>Downloaded</t>
         </is>
       </c>
       <c r="L25" t="inlineStr">
@@ -1688,7 +2000,7 @@
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>Polycab LV IS-7098-I 1C-2XY</t>
+          <t>Polycab LV AL IEC 60502-1 0.6/1kV MC-3 UA</t>
         </is>
       </c>
       <c r="B26" t="inlineStr">
@@ -1698,31 +2010,47 @@
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>IEC 60502-1, IS 7098-1, BS 5467</t>
+          <t>IEC 60502-1</t>
         </is>
       </c>
       <c r="D26" t="inlineStr">
         <is>
-          <t>CE, BIS, CPRI, FQC</t>
-        </is>
-      </c>
-      <c r="E26" t="inlineStr"/>
-      <c r="F26" t="inlineStr"/>
-      <c r="G26" t="inlineStr"/>
+          <t>CE, FQC</t>
+        </is>
+      </c>
+      <c r="E26" t="inlineStr">
+        <is>
+          <t>Higher dielectric strength, Better electrical, mechanical, And thermal properties, UV resistant, Long service life, Low smoke emission</t>
+        </is>
+      </c>
+      <c r="F26" t="inlineStr">
+        <is>
+          <t>Multi core stranded AL conductor, XLPE/EPR/HEPR insulation, Laid up, Inner covering, Armoured, PVC/Polyethylene/Halogen free Outer sheathed LV Cable</t>
+        </is>
+      </c>
+      <c r="G26" t="inlineStr">
+        <is>
+          <t>Multicore stranded Aluminium, XLPE/EPR/HEPR insulation, Laid up, inner covering,PVC/Polyethylene/Halogen free sheathed unarmored Cable suitable for fixed installation such as distribution network or industrial installation.These cables are designed for systems with rated AC voltage 1KV (Um=1.2 KV) between two live conductor.</t>
+        </is>
+      </c>
       <c r="H26" t="inlineStr">
         <is>
-          <t>https://polycab.com/polycab-lv-is-7098-i-1c-2xy/pt-13191/p-54736</t>
-        </is>
-      </c>
-      <c r="I26" t="inlineStr"/>
+          <t>https://polycab.com/polycab-lv-al-iec-60502-1-061kv-mc-3-ua/pt-13191/p-55283</t>
+        </is>
+      </c>
+      <c r="I26" t="inlineStr">
+        <is>
+          <t>polycab_lv_power_cable/images/Polycab_LV_AL_IEC_60502-1_061kV_MC-3_UA_image.png</t>
+        </is>
+      </c>
       <c r="J26" t="inlineStr">
         <is>
-          <t>polycab_lv_power_cable/brochures/Polycab_LV_IS-7098-I_1C-2XY_datasheet.pdf</t>
+          <t>polycab_lv_power_cable/brochures/Polycab_LV_AL_IEC_60502-1_061kV_MC-3_UA_datasheet.pdf</t>
         </is>
       </c>
       <c r="K26" t="inlineStr">
         <is>
-          <t>Not Found</t>
+          <t>Downloaded</t>
         </is>
       </c>
       <c r="L26" t="inlineStr">
@@ -1734,7 +2062,7 @@
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>Polycab LV IS-7098-I 1C-A2XFaY-A2XWaY</t>
+          <t>Polycab LV IS-7098-I 3.5C-2XY</t>
         </is>
       </c>
       <c r="B27" t="inlineStr">
@@ -1744,7 +2072,7 @@
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>IEC 60502-1, IS 7098-1, BS 5467</t>
+          <t>IS 7098-I</t>
         </is>
       </c>
       <c r="D27" t="inlineStr">
@@ -1752,23 +2080,39 @@
           <t>CE, BIS, CPRI, FQC</t>
         </is>
       </c>
-      <c r="E27" t="inlineStr"/>
-      <c r="F27" t="inlineStr"/>
-      <c r="G27" t="inlineStr"/>
+      <c r="E27" t="inlineStr">
+        <is>
+          <t>Higher insulation resistance, Better resistance to surge currents, Low dielectric losses, Long service life, Higher short circuit rating</t>
+        </is>
+      </c>
+      <c r="F27" t="inlineStr">
+        <is>
+          <t>Three and half copper, XLPE Insulation, PVC inner sheathed, unarmoured ,PVC Outer sheathed cable</t>
+        </is>
+      </c>
+      <c r="G27" t="inlineStr">
+        <is>
+          <t>POLYCAB 2XY MC-3.5, Stranded compacted copper conductor, XLPE insulated and PVC sheathed confirming to IS 7098-1 is suitable for AC single phase or three phase (earthed or unearthed) systems with rated voltage up to and including 1100 V. This cable is also suitable for DC systems with rated voltage up to and including 1500 V</t>
+        </is>
+      </c>
       <c r="H27" t="inlineStr">
         <is>
-          <t>https://polycab.com/polycab-lv-is-7098-i-1c-a2xfay-a2xway/pt-13191/p-54734</t>
-        </is>
-      </c>
-      <c r="I27" t="inlineStr"/>
+          <t>https://polycab.com/polycab-lv-is-7098-i-35c-2xy/pt-13191/p-54744</t>
+        </is>
+      </c>
+      <c r="I27" t="inlineStr">
+        <is>
+          <t>polycab_lv_power_cable/images/Polycab_LV_IS-7098-I_35C-2XY_image.png</t>
+        </is>
+      </c>
       <c r="J27" t="inlineStr">
         <is>
-          <t>polycab_lv_power_cable/brochures/Polycab_LV_IS-7098-I_1C-A2XFaY-A2XWaY_datasheet.pdf</t>
+          <t>polycab_lv_power_cable/brochures/Polycab_LV_IS-7098-I_35C-2XY_datasheet.pdf</t>
         </is>
       </c>
       <c r="K27" t="inlineStr">
         <is>
-          <t>Not Found</t>
+          <t>Downloaded</t>
         </is>
       </c>
       <c r="L27" t="inlineStr">
@@ -1780,7 +2124,7 @@
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>Polycab LV IS-7098-I 1C-2XFaY-2XWaY</t>
+          <t>Polycab LV AL IEC 60502-1 0.6/1kV MC-3.5 UA</t>
         </is>
       </c>
       <c r="B28" t="inlineStr">
@@ -1790,31 +2134,47 @@
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>IEC 60502-1, IS 7098-1, BS 5467</t>
+          <t>IEC 60502-1</t>
         </is>
       </c>
       <c r="D28" t="inlineStr">
         <is>
-          <t>CE, BIS, CPRI, FQC</t>
-        </is>
-      </c>
-      <c r="E28" t="inlineStr"/>
-      <c r="F28" t="inlineStr"/>
-      <c r="G28" t="inlineStr"/>
+          <t>CE, FQC</t>
+        </is>
+      </c>
+      <c r="E28" t="inlineStr">
+        <is>
+          <t>Higher dielectric strength, Better electrical, mechanical, And thermal properties, UV resistant, Long service life, Low smoke emission</t>
+        </is>
+      </c>
+      <c r="F28" t="inlineStr">
+        <is>
+          <t>Multi core stranded AL conductor,XLPE/EPR/HEPR insulation, Laid up, Inner covering, Armoured, PVC/Polyethylene/Halogen free Outer sheathed LV Cable</t>
+        </is>
+      </c>
+      <c r="G28" t="inlineStr">
+        <is>
+          <t>Multicore stranded Aluminium, XLPE/EPR/HEPR insulation, Laid up, inner covering,PVC/Polyethylene/Halogen free sheathed unarmored Cable suitable for fixed installation such as distribution network or industrial installation.These cables are designed for systems with rated AC voltage 1KV (Um=1.2 KV) between two live conductor.</t>
+        </is>
+      </c>
       <c r="H28" t="inlineStr">
         <is>
-          <t>https://polycab.com/polycab-lv-is-7098-i-1c-2xfay-2xway/pt-13191/p-54732</t>
-        </is>
-      </c>
-      <c r="I28" t="inlineStr"/>
+          <t>https://polycab.com/polycab-lv-al-iec-60502-1-061kv-mc-35-ua/pt-13191/p-55271</t>
+        </is>
+      </c>
+      <c r="I28" t="inlineStr">
+        <is>
+          <t>polycab_lv_power_cable/images/Polycab_LV_AL_IEC_60502-1_061kV_MC-35_UA_image.png</t>
+        </is>
+      </c>
       <c r="J28" t="inlineStr">
         <is>
-          <t>polycab_lv_power_cable/brochures/Polycab_LV_IS-7098-I_1C-2XFaY-2XWaY_datasheet.pdf</t>
+          <t>polycab_lv_power_cable/brochures/Polycab_LV_AL_IEC_60502-1_061kV_MC-35_UA_datasheet.pdf</t>
         </is>
       </c>
       <c r="K28" t="inlineStr">
         <is>
-          <t>Not Found</t>
+          <t>Downloaded</t>
         </is>
       </c>
       <c r="L28" t="inlineStr">
@@ -1826,7 +2186,7 @@
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>Polycab LV IS-7098-I 4C-A2XY</t>
+          <t>Polycab LV IS-7098-I 3C A2XFY</t>
         </is>
       </c>
       <c r="B29" t="inlineStr">
@@ -1836,7 +2196,7 @@
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>IEC 60502-1, IS 7098-1, BS 5467</t>
+          <t>IS 7098-I</t>
         </is>
       </c>
       <c r="D29" t="inlineStr">
@@ -1844,23 +2204,39 @@
           <t>CE, BIS, CPRI, FQC</t>
         </is>
       </c>
-      <c r="E29" t="inlineStr"/>
-      <c r="F29" t="inlineStr"/>
-      <c r="G29" t="inlineStr"/>
+      <c r="E29" t="inlineStr">
+        <is>
+          <t>Higher Current rating, Higher insulation resistance, Better resistance to surge current, Low dielectric losses, Long service life, Higher short circuit rating</t>
+        </is>
+      </c>
+      <c r="F29" t="inlineStr">
+        <is>
+          <t>Three core aluminium, XLPE Insulation, Inner sheathed &amp; GI flat armoured &amp; PVC Outer sheathed cable</t>
+        </is>
+      </c>
+      <c r="G29" t="inlineStr">
+        <is>
+          <t>POLYCAB A2XFY MC-3, Stranded compacted aluminium conductor, XLPE insulated, PVC inner sheathed, Galvanised Steel Flat strip armour and PVC sheathed confirming to IS 7098-1 is suitable for AC single phase or three phase (earthed or unearthed) systems with rated voltage up to and including 1100 V. This cable is also suitable for DC systems with rated voltage up to and including 1500 V</t>
+        </is>
+      </c>
       <c r="H29" t="inlineStr">
         <is>
-          <t>https://polycab.com/polycab-lv-is-7098-i-4c-a2xy/pt-13191/p-54754</t>
-        </is>
-      </c>
-      <c r="I29" t="inlineStr"/>
+          <t>https://polycab.com/polycab-lv-is-7098-i-3c-a2xfy/pt-13191/p-54720</t>
+        </is>
+      </c>
+      <c r="I29" t="inlineStr">
+        <is>
+          <t>polycab_lv_power_cable/images/Polycab_LV_IS-7098-I_3C_A2XFY_image.png</t>
+        </is>
+      </c>
       <c r="J29" t="inlineStr">
         <is>
-          <t>polycab_lv_power_cable/brochures/Polycab_LV_IS-7098-I_4C-A2XY_datasheet.pdf</t>
+          <t>polycab_lv_power_cable/brochures/Polycab_LV_IS-7098-I_3C_A2XFY_datasheet.pdf</t>
         </is>
       </c>
       <c r="K29" t="inlineStr">
         <is>
-          <t>Not Found</t>
+          <t>Downloaded</t>
         </is>
       </c>
       <c r="L29" t="inlineStr">
@@ -1872,7 +2248,7 @@
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>Polycab LV AL IEC 60502-1 0.6/1kV MC-4 UA</t>
+          <t>Polycab LV IS-7098-I 3C-2XY</t>
         </is>
       </c>
       <c r="B30" t="inlineStr">
@@ -1882,35 +2258,47 @@
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>IEC 60502-1, BS 5467</t>
+          <t>IS 7098-I</t>
         </is>
       </c>
       <c r="D30" t="inlineStr">
         <is>
-          <t>CE, FQC</t>
+          <t>CE, BIS, CPRI, FQC</t>
         </is>
       </c>
       <c r="E30" t="inlineStr">
         <is>
-          <t>UV Resistant, Low Smoke</t>
-        </is>
-      </c>
-      <c r="F30" t="inlineStr"/>
-      <c r="G30" t="inlineStr"/>
+          <t>Higher insulation resistance, Better resistance to surge currents, Low dielectric losses, Long service life, Higher short circuit rating</t>
+        </is>
+      </c>
+      <c r="F30" t="inlineStr">
+        <is>
+          <t>Three core copper, XLPE Insulation, PVC inner sheathed, unarmoured ,PVC Outer sheathed cable</t>
+        </is>
+      </c>
+      <c r="G30" t="inlineStr">
+        <is>
+          <t>POLYCAB 2XY MC-3, Stranded compacted copper conductor, XLPE insulated and PVC sheathed confirming to IS 7098-1 is suitable for AC single phase or three phase (earthed or unearthed) systems with rated voltage up to and including 1100 V. This cable is also suitable for DC systems with rated voltage up to and including 1500 V</t>
+        </is>
+      </c>
       <c r="H30" t="inlineStr">
         <is>
-          <t>https://polycab.com/polycab-lv-al-iec-60502-1-061kv-mc-4-ua/pt-13191/p-55295</t>
-        </is>
-      </c>
-      <c r="I30" t="inlineStr"/>
+          <t>https://polycab.com/polycab-lv-is-7098-i-3c-2xy/pt-13191/p-54748</t>
+        </is>
+      </c>
+      <c r="I30" t="inlineStr">
+        <is>
+          <t>polycab_lv_power_cable/images/Polycab_LV_IS-7098-I_3C-2XY_image.png</t>
+        </is>
+      </c>
       <c r="J30" t="inlineStr">
         <is>
-          <t>polycab_lv_power_cable/brochures/Polycab_LV_AL_IEC_60502-1_061kV_MC-4_UA_datasheet.pdf</t>
+          <t>polycab_lv_power_cable/brochures/Polycab_LV_IS-7098-I_3C-2XY_datasheet.pdf</t>
         </is>
       </c>
       <c r="K30" t="inlineStr">
         <is>
-          <t>Not Found</t>
+          <t>Downloaded</t>
         </is>
       </c>
       <c r="L30" t="inlineStr">
@@ -1922,7 +2310,7 @@
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>Polycab LV Cu IEC 60502-1 0.6/1kV MC-3 SFA</t>
+          <t>Polycab LV IS-7098-I 4C-A2XY</t>
         </is>
       </c>
       <c r="B31" t="inlineStr">
@@ -1932,35 +2320,47 @@
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>IEC 60502-1, BS 5467</t>
+          <t>IS 7098-I</t>
         </is>
       </c>
       <c r="D31" t="inlineStr">
         <is>
-          <t>CE, FQC</t>
+          <t>CE, BIS, CPRI, FQC</t>
         </is>
       </c>
       <c r="E31" t="inlineStr">
         <is>
-          <t>UV Resistant, Low Smoke</t>
-        </is>
-      </c>
-      <c r="F31" t="inlineStr"/>
-      <c r="G31" t="inlineStr"/>
+          <t>Higher insulation resistance, Better resistance to surge currents, Low dielectric losses, Long service life, Higher short circuit rating</t>
+        </is>
+      </c>
+      <c r="F31" t="inlineStr">
+        <is>
+          <t>Four core Aluminium, XLPE Insulation, PVC inner sheathed, unarmoured, PVC Outer sheathed cable</t>
+        </is>
+      </c>
+      <c r="G31" t="inlineStr">
+        <is>
+          <t>POLYCAB A2XY MC-4, Stranded compacted aluminium conductor, XLPE insulated, and PVC sheathed confirming to IS 7098-1 is suitable for AC single phase or three phase (earthed or unearthed) systems with rated voltage up to and including 1100 V. This cable is also suitable for DC systems with rated voltage up to and including 1500 V</t>
+        </is>
+      </c>
       <c r="H31" t="inlineStr">
         <is>
-          <t>https://polycab.com/polycab-lv-cu-iec-60502-1-061kv-mc-3-sfa/pt-13191/p-55285</t>
-        </is>
-      </c>
-      <c r="I31" t="inlineStr"/>
+          <t>https://polycab.com/polycab-lv-is-7098-i-4c-a2xy/pt-13191/p-54754</t>
+        </is>
+      </c>
+      <c r="I31" t="inlineStr">
+        <is>
+          <t>polycab_lv_power_cable/images/Polycab_LV_IS-7098-I_4C-A2XY_image.png</t>
+        </is>
+      </c>
       <c r="J31" t="inlineStr">
         <is>
-          <t>polycab_lv_power_cable/brochures/Polycab_LV_Cu_IEC_60502-1_061kV_MC-3_SFA_datasheet.pdf</t>
+          <t>polycab_lv_power_cable/brochures/Polycab_LV_IS-7098-I_4C-A2XY_datasheet.pdf</t>
         </is>
       </c>
       <c r="K31" t="inlineStr">
         <is>
-          <t>Not Found</t>
+          <t>Downloaded</t>
         </is>
       </c>
       <c r="L31" t="inlineStr">
@@ -1972,7 +2372,7 @@
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>Polycab LV IS-7098-I 3.5C 2XFY</t>
+          <t>Polycab LV Cu IEC 60502-1 0.6/1kV MC-2 SWA</t>
         </is>
       </c>
       <c r="B32" t="inlineStr">
@@ -1982,31 +2382,47 @@
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>IEC 60502-1, IS 7098-1, BS 5467</t>
+          <t>IEC 60502-1</t>
         </is>
       </c>
       <c r="D32" t="inlineStr">
         <is>
-          <t>CE, BIS, CPRI, FQC</t>
-        </is>
-      </c>
-      <c r="E32" t="inlineStr"/>
-      <c r="F32" t="inlineStr"/>
-      <c r="G32" t="inlineStr"/>
+          <t>CE, FQC</t>
+        </is>
+      </c>
+      <c r="E32" t="inlineStr">
+        <is>
+          <t>Higher dielectric strength, Better electrical, mechanical, And thermal properties, UV resistant, Long service life, Low smoke emission</t>
+        </is>
+      </c>
+      <c r="F32" t="inlineStr">
+        <is>
+          <t>Multi core stranded copper conductor, XLPE/EPR/HEPR insulation, Laid up, Inner covering, Armoured, PVC/Polyethylene/Halogen free Outer sheathed LV Cable</t>
+        </is>
+      </c>
+      <c r="G32" t="inlineStr">
+        <is>
+          <t>Multicore stranded Copper, XLPE/EPR/HEPR insulation, Laid up, inner covering GI wire armored,PVC/Polyethylene/Halogen free sheathed Cable suitable for fixed installation such as distribution network or industrial installation.These cables are designed for systems with rated AC voltage 1KV (Um=1.2 KV) between two live conductor.</t>
+        </is>
+      </c>
       <c r="H32" t="inlineStr">
         <is>
-          <t>https://polycab.com/polycab-lv-is-7098-i-35c-2xfy/pt-13191/p-54708</t>
-        </is>
-      </c>
-      <c r="I32" t="inlineStr"/>
+          <t>https://polycab.com/polycab-lv-cu-iec-60502-1-061kv-mc-2-swa/pt-13191/p-55263</t>
+        </is>
+      </c>
+      <c r="I32" t="inlineStr">
+        <is>
+          <t>polycab_lv_power_cable/images/Polycab_LV_Cu_IEC_60502-1_061kV_MC-2_SWA_image.png</t>
+        </is>
+      </c>
       <c r="J32" t="inlineStr">
         <is>
-          <t>polycab_lv_power_cable/brochures/Polycab_LV_IS-7098-I_35C_2XFY_datasheet.pdf</t>
+          <t>polycab_lv_power_cable/brochures/Polycab_LV_Cu_IEC_60502-1_061kV_MC-2_SWA_datasheet.pdf</t>
         </is>
       </c>
       <c r="K32" t="inlineStr">
         <is>
-          <t>Not Found</t>
+          <t>Downloaded</t>
         </is>
       </c>
       <c r="L32" t="inlineStr">
@@ -2018,7 +2434,7 @@
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>Polycab LV AL IEC 60502-1 0.6/1kV MC-3 SFA</t>
+          <t>Polycab LV Cu IEC 60502-1 0.6/1kV MC-3 UA</t>
         </is>
       </c>
       <c r="B33" t="inlineStr">
@@ -2028,7 +2444,7 @@
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>IEC 60502-1, BS 5467</t>
+          <t>IEC 60502-1</t>
         </is>
       </c>
       <c r="D33" t="inlineStr">
@@ -2038,25 +2454,37 @@
       </c>
       <c r="E33" t="inlineStr">
         <is>
-          <t>UV Resistant, Low Smoke</t>
-        </is>
-      </c>
-      <c r="F33" t="inlineStr"/>
-      <c r="G33" t="inlineStr"/>
+          <t>Higher dielectric strength, Better electrical, mechanical, And thermal properties, UV resistant, Long service life, Low smoke emission</t>
+        </is>
+      </c>
+      <c r="F33" t="inlineStr">
+        <is>
+          <t>Multi core stranded copper conductor,XLPE/EPR/HEPR insulation, Laid up, Inner covering, Armoured, PVC/Polyethylene/Halogen frer Outer sheathed LV Cable</t>
+        </is>
+      </c>
+      <c r="G33" t="inlineStr">
+        <is>
+          <t>Multicore stranded Copper, XLPE/EPR/HEPR insulation, Laid up, inner covering,PVC/Polyethylene/Halogen free sheathed unarmored Cable suitable for fixed installation such as distribution network or industrial installation.These cables are designed for systems with rated AC voltage 1KV (Um=1.2 KV) between two live conductor.</t>
+        </is>
+      </c>
       <c r="H33" t="inlineStr">
         <is>
-          <t>https://polycab.com/polycab-lv-al-iec-60502-1-061kv-mc-3-sfa/pt-13191/p-55279</t>
-        </is>
-      </c>
-      <c r="I33" t="inlineStr"/>
+          <t>https://polycab.com/polycab-lv-cu-iec-60502-1-061kv-mc-3-ua/pt-13191/p-55289</t>
+        </is>
+      </c>
+      <c r="I33" t="inlineStr">
+        <is>
+          <t>polycab_lv_power_cable/images/Polycab_LV_Cu_IEC_60502-1_061kV_MC-3_UA_image.png</t>
+        </is>
+      </c>
       <c r="J33" t="inlineStr">
         <is>
-          <t>polycab_lv_power_cable/brochures/Polycab_LV_AL_IEC_60502-1_061kV_MC-3_SFA_datasheet.pdf</t>
+          <t>polycab_lv_power_cable/brochures/Polycab_LV_Cu_IEC_60502-1_061kV_MC-3_UA_datasheet.pdf</t>
         </is>
       </c>
       <c r="K33" t="inlineStr">
         <is>
-          <t>Not Found</t>
+          <t>Downloaded</t>
         </is>
       </c>
       <c r="L33" t="inlineStr">
@@ -2068,7 +2496,7 @@
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>Polycab LV IS-7098-I 3C 2XWY</t>
+          <t>Polycab LV IS-7098-I 4C 2XWY</t>
         </is>
       </c>
       <c r="B34" t="inlineStr">
@@ -2078,7 +2506,7 @@
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>IEC 60502-1, IS 7098-1, BS 5467</t>
+          <t>IS 7098-I</t>
         </is>
       </c>
       <c r="D34" t="inlineStr">
@@ -2086,23 +2514,39 @@
           <t>CE, BIS, CPRI, FQC</t>
         </is>
       </c>
-      <c r="E34" t="inlineStr"/>
-      <c r="F34" t="inlineStr"/>
-      <c r="G34" t="inlineStr"/>
+      <c r="E34" t="inlineStr">
+        <is>
+          <t>Higher Current rating, Higher insulation resistance, Better resistance to surge current, Low dielectric losses, Long service life, Higher short circuit rating</t>
+        </is>
+      </c>
+      <c r="F34" t="inlineStr">
+        <is>
+          <t>Four core copper, XLPE Insulation, Inner sheathed &amp; GI round armoured &amp; PVC Outer sheathed cable</t>
+        </is>
+      </c>
+      <c r="G34" t="inlineStr">
+        <is>
+          <t>POLYCAB 2XWY MC-4, Stranded compacted copper conductor, XLPE insulated, PVC inner sheathed, Galvanised Steel round wire armour and PVC sheathed confirming to IS 7098-1 is suitable for AC single phase or three phase (earthed or unearthed) systems with rated voltage up to and including 1100 V. This cable is also suitable for DC systems with rated voltage up to and including 1500 V</t>
+        </is>
+      </c>
       <c r="H34" t="inlineStr">
         <is>
-          <t>https://polycab.com/polycab-lv-is-7098-i-3c-2xwy/pt-13191/p-54718</t>
-        </is>
-      </c>
-      <c r="I34" t="inlineStr"/>
+          <t>https://polycab.com/polycab-lv-is-7098-i-4c-2xwy/pt-13191/p-54726</t>
+        </is>
+      </c>
+      <c r="I34" t="inlineStr">
+        <is>
+          <t>polycab_lv_power_cable/images/Polycab_LV_IS-7098-I_4C_2XWY_image.png</t>
+        </is>
+      </c>
       <c r="J34" t="inlineStr">
         <is>
-          <t>polycab_lv_power_cable/brochures/Polycab_LV_IS-7098-I_3C_2XWY_datasheet.pdf</t>
+          <t>polycab_lv_power_cable/brochures/Polycab_LV_IS-7098-I_4C_2XWY_datasheet.pdf</t>
         </is>
       </c>
       <c r="K34" t="inlineStr">
         <is>
-          <t>Not Found</t>
+          <t>Downloaded</t>
         </is>
       </c>
       <c r="L34" t="inlineStr">
@@ -2114,7 +2558,7 @@
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>Polycab LV AL IEC 60502-1 0.6/1kV MC-4 SWA</t>
+          <t>Polycab LV Cu IEC 60502-1 0.6/1kV SC UA</t>
         </is>
       </c>
       <c r="B35" t="inlineStr">
@@ -2124,7 +2568,7 @@
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>IEC 60502-1, BS 5467</t>
+          <t>IEC 60502-1</t>
         </is>
       </c>
       <c r="D35" t="inlineStr">
@@ -2134,25 +2578,37 @@
       </c>
       <c r="E35" t="inlineStr">
         <is>
-          <t>UV Resistant, Low Smoke</t>
-        </is>
-      </c>
-      <c r="F35" t="inlineStr"/>
-      <c r="G35" t="inlineStr"/>
+          <t>Higher dielectric strength, Better electrical, mechanical, And thermal properties, UV resistant, Long service life, Low smoke emission</t>
+        </is>
+      </c>
+      <c r="F35" t="inlineStr">
+        <is>
+          <t>Single core stranded copper conductor,XLPE/EPR/HEPR insulation, unarmoured,PVC/Polyethylene/Halogen free Outer sheathed LV Cable</t>
+        </is>
+      </c>
+      <c r="G35" t="inlineStr">
+        <is>
+          <t>Single core stranded Copper conductor, XLPE/EPR/HEPR insulation,PVC/Polyethylene/Halogen free Inner &amp; outer sheathed Cable. suitable for fixed installation such as distribution network or industrial installation. These cable cables are designed for systems with rated AC voltage 1KV (Um=1.2 KV).</t>
+        </is>
+      </c>
       <c r="H35" t="inlineStr">
         <is>
-          <t>https://polycab.com/polycab-lv-al-iec-60502-1-061kv-mc-4-swa/pt-13191/p-55293</t>
-        </is>
-      </c>
-      <c r="I35" t="inlineStr"/>
+          <t>https://polycab.com/polycab-lv-cu-iec-60502-1-061kv-sc-ua/pt-13191/p-55253</t>
+        </is>
+      </c>
+      <c r="I35" t="inlineStr">
+        <is>
+          <t>polycab_lv_power_cable/images/Polycab_LV_Cu_IEC_60502-1_061kV_SC_UA_image.png</t>
+        </is>
+      </c>
       <c r="J35" t="inlineStr">
         <is>
-          <t>polycab_lv_power_cable/brochures/Polycab_LV_AL_IEC_60502-1_061kV_MC-4_SWA_datasheet.pdf</t>
+          <t>polycab_lv_power_cable/brochures/Polycab_LV_Cu_IEC_60502-1_061kV_SC_UA_datasheet.pdf</t>
         </is>
       </c>
       <c r="K35" t="inlineStr">
         <is>
-          <t>Not Found</t>
+          <t>Downloaded</t>
         </is>
       </c>
       <c r="L35" t="inlineStr">
@@ -2174,7 +2630,7 @@
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>IEC 60502-1, IS 7098-1, BS 5467</t>
+          <t>IS 7098-I</t>
         </is>
       </c>
       <c r="D36" t="inlineStr">
@@ -2182,15 +2638,31 @@
           <t>CE, BIS, CPRI, FQC</t>
         </is>
       </c>
-      <c r="E36" t="inlineStr"/>
-      <c r="F36" t="inlineStr"/>
-      <c r="G36" t="inlineStr"/>
+      <c r="E36" t="inlineStr">
+        <is>
+          <t>Higher Current rating, Higher insulation resistance, Better resistance to surge current, Low dielectric losses, Long service life, Higher short circuit rating</t>
+        </is>
+      </c>
+      <c r="F36" t="inlineStr">
+        <is>
+          <t>Three and half core Aluminium conductor, XLPE Insulation, Inner sheathed &amp; GI round armoured &amp; PVC Outer sheathed cable</t>
+        </is>
+      </c>
+      <c r="G36" t="inlineStr">
+        <is>
+          <t>POLYCAB A2XWY MC-3.5, Stranded compacted aluminium conductor, XLPE insulated, PVC inner sheathed Galvanised Steel round wire armour and PVC sheathed confirming to IS 7098-1 is suitable for AC single phase or three phase (earthed or unearthed) systems with rated voltage up to and including 1100 V. This cable is also suitable for DC systems with rated voltage up to and including 1500 V</t>
+        </is>
+      </c>
       <c r="H36" t="inlineStr">
         <is>
           <t>https://polycab.com/polycab-lv-is-7098-i-35c-a2xwy/pt-13191/p-54714</t>
         </is>
       </c>
-      <c r="I36" t="inlineStr"/>
+      <c r="I36" t="inlineStr">
+        <is>
+          <t>polycab_lv_power_cable/images/Polycab_LV_IS-7098-I_35C_A2XWY_image.png</t>
+        </is>
+      </c>
       <c r="J36" t="inlineStr">
         <is>
           <t>polycab_lv_power_cable/brochures/Polycab_LV_IS-7098-I_35C_A2XWY_datasheet.pdf</t>
@@ -2198,7 +2670,7 @@
       </c>
       <c r="K36" t="inlineStr">
         <is>
-          <t>Not Found</t>
+          <t>Downloaded</t>
         </is>
       </c>
       <c r="L36" t="inlineStr">
@@ -2210,7 +2682,7 @@
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>Polycab LV IS-7098-I 4C-2XY</t>
+          <t>Polycab LV IS-7098-I 4C A2XFY</t>
         </is>
       </c>
       <c r="B37" t="inlineStr">
@@ -2220,7 +2692,7 @@
       </c>
       <c r="C37" t="inlineStr">
         <is>
-          <t>IEC 60502-1, IS 7098-1, BS 5467</t>
+          <t>IS 7098-I</t>
         </is>
       </c>
       <c r="D37" t="inlineStr">
@@ -2228,23 +2700,39 @@
           <t>CE, BIS, CPRI, FQC</t>
         </is>
       </c>
-      <c r="E37" t="inlineStr"/>
-      <c r="F37" t="inlineStr"/>
-      <c r="G37" t="inlineStr"/>
+      <c r="E37" t="inlineStr">
+        <is>
+          <t>Higher Current rating, Higher insulation resistance, Better resistance to surge current, Low dielectric losses, Long service life, Higher short circuit rating</t>
+        </is>
+      </c>
+      <c r="F37" t="inlineStr">
+        <is>
+          <t>Four core Aluminium, XLPE Insulation, Inner sheathed &amp; GI flat armoured &amp; PVC Outer sheathed cable</t>
+        </is>
+      </c>
+      <c r="G37" t="inlineStr">
+        <is>
+          <t>POLYCAB A2XFY MC-4, Stranded compacted aluminium conductor, XLPE insulated, PVC inner sheathed, Galvanised Steel Flat strip armour and PVC sheathed confirming to IS 7098-1 is suitable for AC single phase or three phase (earthed or unearthed) systems with rated voltage up to and including 1100 V. This cable is also suitable for DC systems with rated voltage up to and including 1500 V</t>
+        </is>
+      </c>
       <c r="H37" t="inlineStr">
         <is>
-          <t>https://polycab.com/polycab-lv-is-7098-i-4c-2xy/pt-13191/p-54752</t>
-        </is>
-      </c>
-      <c r="I37" t="inlineStr"/>
+          <t>https://polycab.com/polycab-lv-is-7098-i-4c-a2xfy/pt-13191/p-54728</t>
+        </is>
+      </c>
+      <c r="I37" t="inlineStr">
+        <is>
+          <t>polycab_lv_power_cable/images/Polycab_LV_IS-7098-I_4C_A2XFY_image.png</t>
+        </is>
+      </c>
       <c r="J37" t="inlineStr">
         <is>
-          <t>polycab_lv_power_cable/brochures/Polycab_LV_IS-7098-I_4C-2XY_datasheet.pdf</t>
+          <t>polycab_lv_power_cable/brochures/Polycab_LV_IS-7098-I_4C_A2XFY_datasheet.pdf</t>
         </is>
       </c>
       <c r="K37" t="inlineStr">
         <is>
-          <t>Not Found</t>
+          <t>Downloaded</t>
         </is>
       </c>
       <c r="L37" t="inlineStr">
@@ -2256,7 +2744,7 @@
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>Polycab LV IS-7098-I 3.5C-2XY</t>
+          <t>Polycab LV AL IEC 60502-1 0.6/1kV MC-3 SWA</t>
         </is>
       </c>
       <c r="B38" t="inlineStr">
@@ -2266,31 +2754,47 @@
       </c>
       <c r="C38" t="inlineStr">
         <is>
-          <t>IEC 60502-1, IS 7098-1, BS 5467</t>
+          <t>IEC 60502-1</t>
         </is>
       </c>
       <c r="D38" t="inlineStr">
         <is>
-          <t>CE, BIS, CPRI, FQC</t>
-        </is>
-      </c>
-      <c r="E38" t="inlineStr"/>
-      <c r="F38" t="inlineStr"/>
-      <c r="G38" t="inlineStr"/>
+          <t>CE, FQC</t>
+        </is>
+      </c>
+      <c r="E38" t="inlineStr">
+        <is>
+          <t>Higher dielectric strength, Better electrical, mechanical, And thermal properties, UV resistant, Long service life, Low smoke emission</t>
+        </is>
+      </c>
+      <c r="F38" t="inlineStr">
+        <is>
+          <t>Multi core stranded AL conductor, XLPE insulation, Laid up, Inner covering, Armoured, PVC/Polyethylene/Halogen free Outer sheathed LV Cable</t>
+        </is>
+      </c>
+      <c r="G38" t="inlineStr">
+        <is>
+          <t>Multicore stranded Aluminium, XLPE/EPR/HEPR insulation, Laid up, inner covering,GI wire,PVC/Polyethylene/Halogen free sheathed Cable suitable for fixed installation such as distribution network or industrial installation.These cables are designed for systems with rated AC voltage 1KV (Um=1.2 KV) between two live conductor.</t>
+        </is>
+      </c>
       <c r="H38" t="inlineStr">
         <is>
-          <t>https://polycab.com/polycab-lv-is-7098-i-35c-2xy/pt-13191/p-54744</t>
-        </is>
-      </c>
-      <c r="I38" t="inlineStr"/>
+          <t>https://polycab.com/polycab-lv-al-iec-60502-1-061kv-mc-3-swa/pt-13191/p-55281</t>
+        </is>
+      </c>
+      <c r="I38" t="inlineStr">
+        <is>
+          <t>polycab_lv_power_cable/images/Polycab_LV_AL_IEC_60502-1_061kV_MC-3_SWA_image.png</t>
+        </is>
+      </c>
       <c r="J38" t="inlineStr">
         <is>
-          <t>polycab_lv_power_cable/brochures/Polycab_LV_IS-7098-I_35C-2XY_datasheet.pdf</t>
+          <t>polycab_lv_power_cable/brochures/Polycab_LV_AL_IEC_60502-1_061kV_MC-3_SWA_datasheet.pdf</t>
         </is>
       </c>
       <c r="K38" t="inlineStr">
         <is>
-          <t>Not Found</t>
+          <t>Downloaded</t>
         </is>
       </c>
       <c r="L38" t="inlineStr">
@@ -2302,7 +2806,7 @@
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>Polycab LV AL IEC 60502-1 0.6/1kV MC-2 UA</t>
+          <t>Polycab LV IS-7098-I 3.5C A2XFY</t>
         </is>
       </c>
       <c r="B39" t="inlineStr">
@@ -2312,35 +2816,47 @@
       </c>
       <c r="C39" t="inlineStr">
         <is>
-          <t>IEC 60502-1, BS 5467</t>
+          <t>IS 7098-I</t>
         </is>
       </c>
       <c r="D39" t="inlineStr">
         <is>
-          <t>CE, FQC</t>
+          <t>CE, BIS, CPRI, FQC</t>
         </is>
       </c>
       <c r="E39" t="inlineStr">
         <is>
-          <t>UV Resistant, Low Smoke</t>
-        </is>
-      </c>
-      <c r="F39" t="inlineStr"/>
-      <c r="G39" t="inlineStr"/>
+          <t>Higher Current rating, Higher insulation resistance, Better resistance to surge current, Low dielectric losses, Long service life, Higher short circuit rating</t>
+        </is>
+      </c>
+      <c r="F39" t="inlineStr">
+        <is>
+          <t>Three and half core Aluminium conductor, XLPE Insulation Inner sheathed &amp; GI flat armoured &amp; PVC Outer sheathed cable</t>
+        </is>
+      </c>
+      <c r="G39" t="inlineStr">
+        <is>
+          <t>POLYCAB A2XFY MC-3.5,Stranded compacted aluminium conductor ,XLPE insulated, PVC inner sheathed, Galvanised Steel Flat strip armour and PVC sheathed confirming to IS 7098-1 is suitable for AC single phase or three phase (earthed or unearthed) systems with rated voltage up to and including 1100 V. This cable is also suitable for DC systems with rated voltage up to and including 1500 V</t>
+        </is>
+      </c>
       <c r="H39" t="inlineStr">
         <is>
-          <t>https://polycab.com/polycab-lv-al-iec-60502-1-061kv-mc-2-ua/pt-13191/p-55259</t>
-        </is>
-      </c>
-      <c r="I39" t="inlineStr"/>
+          <t>https://polycab.com/polycab-lv-is-7098-i-35c-a2xfy/pt-13191/p-54712</t>
+        </is>
+      </c>
+      <c r="I39" t="inlineStr">
+        <is>
+          <t>polycab_lv_power_cable/images/Polycab_LV_IS-7098-I_35C_A2XFY_image.png</t>
+        </is>
+      </c>
       <c r="J39" t="inlineStr">
         <is>
-          <t>polycab_lv_power_cable/brochures/Polycab_LV_AL_IEC_60502-1_061kV_MC-2_UA_datasheet.pdf</t>
+          <t>polycab_lv_power_cable/brochures/Polycab_LV_IS-7098-I_35C_A2XFY_datasheet.pdf</t>
         </is>
       </c>
       <c r="K39" t="inlineStr">
         <is>
-          <t>Not Found</t>
+          <t>Downloaded</t>
         </is>
       </c>
       <c r="L39" t="inlineStr">
@@ -2352,7 +2868,7 @@
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>Polycab BS 6724 SC AWA LSZH 0.6/1kV AC</t>
+          <t>Polycab LV Cu IEC 60502-1 0.6/1kV MC-2 SFA</t>
         </is>
       </c>
       <c r="B40" t="inlineStr">
@@ -2362,7 +2878,7 @@
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t>IEC 60502-1, BS 6724, BS 5467</t>
+          <t>IEC 60502-1</t>
         </is>
       </c>
       <c r="D40" t="inlineStr">
@@ -2372,25 +2888,37 @@
       </c>
       <c r="E40" t="inlineStr">
         <is>
-          <t>High Life, Low Smoke</t>
-        </is>
-      </c>
-      <c r="F40" t="inlineStr"/>
-      <c r="G40" t="inlineStr"/>
+          <t>Higher dielectric strength, Better electrical, mechanical, And thermal properties, UV resistant, Long service life, Low smoke emission</t>
+        </is>
+      </c>
+      <c r="F40" t="inlineStr">
+        <is>
+          <t>Multi core stranded copper conductor, XLPE/EPR/HEPR insulation, Laid up, Inner covering, Armoured, PVC/Polyethylene/Halogen free Outer sheathed LV Cable</t>
+        </is>
+      </c>
+      <c r="G40" t="inlineStr">
+        <is>
+          <t>Multicore stranded Copper, XLPE/EPR/HEPR insulation, Laid up, inner covering GI flat strip armored,PVC/Polyethylene/Halogen free sheathed Cable suitable for fixed installation such as distribution network or industrial installation.These cables are designed for systems with rated AC voltage 1KV (Um=1.2 KV) between two live conductor.</t>
+        </is>
+      </c>
       <c r="H40" t="inlineStr">
         <is>
-          <t>https://polycab.com/polycab-bs-6724-sc-awa-lszh-061kv-ac/pt-13191/p-55455</t>
-        </is>
-      </c>
-      <c r="I40" t="inlineStr"/>
+          <t>https://polycab.com/polycab-lv-cu-iec-60502-1-061kv-mc-2-sfa/pt-13191/p-55261</t>
+        </is>
+      </c>
+      <c r="I40" t="inlineStr">
+        <is>
+          <t>polycab_lv_power_cable/images/Polycab_LV_Cu_IEC_60502-1_061kV_MC-2_SFA_image.png</t>
+        </is>
+      </c>
       <c r="J40" t="inlineStr">
         <is>
-          <t>polycab_lv_power_cable/brochures/Polycab_BS_6724_SC_AWA_LSZH_061kV_AC_datasheet.pdf</t>
+          <t>polycab_lv_power_cable/brochures/Polycab_LV_Cu_IEC_60502-1_061kV_MC-2_SFA_datasheet.pdf</t>
         </is>
       </c>
       <c r="K40" t="inlineStr">
         <is>
-          <t>Not Found</t>
+          <t>Downloaded</t>
         </is>
       </c>
       <c r="L40" t="inlineStr">
@@ -2402,7 +2930,7 @@
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>Polycab LV IS-7098-I 3.5C 2XWY</t>
+          <t>Polycab LV IS-7098-I 3.5C-A2XY</t>
         </is>
       </c>
       <c r="B41" t="inlineStr">
@@ -2412,7 +2940,7 @@
       </c>
       <c r="C41" t="inlineStr">
         <is>
-          <t>IEC 60502-1, IS 7098-1, BS 5467</t>
+          <t>IS 7098-I</t>
         </is>
       </c>
       <c r="D41" t="inlineStr">
@@ -2420,23 +2948,39 @@
           <t>CE, BIS, CPRI, FQC</t>
         </is>
       </c>
-      <c r="E41" t="inlineStr"/>
-      <c r="F41" t="inlineStr"/>
-      <c r="G41" t="inlineStr"/>
+      <c r="E41" t="inlineStr">
+        <is>
+          <t>Higher insulation resistance, Better resistance to surge currents, Low dielectric losses, Long service life, Higher short circuit rating</t>
+        </is>
+      </c>
+      <c r="F41" t="inlineStr">
+        <is>
+          <t>Three and half Aluminium, XLPE Insulation, PVC inner sheathed, unarmoured ,PVC Outer sheathed cable</t>
+        </is>
+      </c>
+      <c r="G41" t="inlineStr">
+        <is>
+          <t>POLYCAB A2XY MC-3.5, Stranded compacted aluminium conductor, XLPE insulated, and PVC sheathed confirming to IS 7098-1 is suitable for AC single phase or three phase (earthed or unearthed) systems with rated voltage up to and including 1100 V. This cable is also suitable for DC systems with rated voltage up to and including 1500 V</t>
+        </is>
+      </c>
       <c r="H41" t="inlineStr">
         <is>
-          <t>https://polycab.com/polycab-lv-is-7098-i-35c-2xwy/pt-13191/p-54710</t>
-        </is>
-      </c>
-      <c r="I41" t="inlineStr"/>
+          <t>https://polycab.com/polycab-lv-is-7098-i-35c-a2xy/pt-13191/p-54746</t>
+        </is>
+      </c>
+      <c r="I41" t="inlineStr">
+        <is>
+          <t>polycab_lv_power_cable/images/Polycab_LV_IS-7098-I_35C-A2XY_image.png</t>
+        </is>
+      </c>
       <c r="J41" t="inlineStr">
         <is>
-          <t>polycab_lv_power_cable/brochures/Polycab_LV_IS-7098-I_35C_2XWY_datasheet.pdf</t>
+          <t>polycab_lv_power_cable/brochures/Polycab_LV_IS-7098-I_35C-A2XY_datasheet.pdf</t>
         </is>
       </c>
       <c r="K41" t="inlineStr">
         <is>
-          <t>Not Found</t>
+          <t>Downloaded</t>
         </is>
       </c>
       <c r="L41" t="inlineStr">
@@ -2448,7 +2992,7 @@
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>Polycab LV AL IEC 60502-1 0.6/1kV MC-3 UA</t>
+          <t>Polycab LV IS-7098-I 2C-2XY</t>
         </is>
       </c>
       <c r="B42" t="inlineStr">
@@ -2458,35 +3002,47 @@
       </c>
       <c r="C42" t="inlineStr">
         <is>
-          <t>IEC 60502-1, BS 5467</t>
+          <t>IS 7098-I</t>
         </is>
       </c>
       <c r="D42" t="inlineStr">
         <is>
-          <t>CE, FQC</t>
+          <t>CE, BIS, CPRI, FQC</t>
         </is>
       </c>
       <c r="E42" t="inlineStr">
         <is>
-          <t>UV Resistant, Low Smoke</t>
-        </is>
-      </c>
-      <c r="F42" t="inlineStr"/>
-      <c r="G42" t="inlineStr"/>
+          <t>Higher insulation resistance, Better resistance to surge currents, Low dielectric losses, Long service life, Higher short circuit rating</t>
+        </is>
+      </c>
+      <c r="F42" t="inlineStr">
+        <is>
+          <t>Two core copper, XLPE Insulation, PVC inner sheathed, unarmoured ,PVC Outer sheathed cable</t>
+        </is>
+      </c>
+      <c r="G42" t="inlineStr">
+        <is>
+          <t>POLYCAB 2XY MC-2, Stranded compacted copper conductor, XLPE insulated, and PVC sheathed confirming to IS 7098-1 is suitable for AC single phase or three phase (earthed or unearthed) systems with rated voltage up to and including 1100 V. This cable is also suitable for DC systems with rated voltage up to and including 1500 V</t>
+        </is>
+      </c>
       <c r="H42" t="inlineStr">
         <is>
-          <t>https://polycab.com/polycab-lv-al-iec-60502-1-061kv-mc-3-ua/pt-13191/p-55283</t>
-        </is>
-      </c>
-      <c r="I42" t="inlineStr"/>
+          <t>https://polycab.com/polycab-lv-is-7098-i-2c-2xy/pt-13191/p-54740</t>
+        </is>
+      </c>
+      <c r="I42" t="inlineStr">
+        <is>
+          <t>polycab_lv_power_cable/images/Polycab_LV_IS-7098-I_2C-2XY_image.png</t>
+        </is>
+      </c>
       <c r="J42" t="inlineStr">
         <is>
-          <t>polycab_lv_power_cable/brochures/Polycab_LV_AL_IEC_60502-1_061kV_MC-3_UA_datasheet.pdf</t>
+          <t>polycab_lv_power_cable/brochures/Polycab_LV_IS-7098-I_2C-2XY_datasheet.pdf</t>
         </is>
       </c>
       <c r="K42" t="inlineStr">
         <is>
-          <t>Not Found</t>
+          <t>Downloaded</t>
         </is>
       </c>
       <c r="L42" t="inlineStr">
@@ -2498,7 +3054,7 @@
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>Polycab LV IS-7098-I 3.5C-A2XY</t>
+          <t>Polycab LV IS-7098-I 1C-A2XFaY-A2XWaY</t>
         </is>
       </c>
       <c r="B43" t="inlineStr">
@@ -2508,7 +3064,7 @@
       </c>
       <c r="C43" t="inlineStr">
         <is>
-          <t>IEC 60502-1, IS 7098-1, BS 5467</t>
+          <t>IS 7098-I</t>
         </is>
       </c>
       <c r="D43" t="inlineStr">
@@ -2516,23 +3072,39 @@
           <t>CE, BIS, CPRI, FQC</t>
         </is>
       </c>
-      <c r="E43" t="inlineStr"/>
-      <c r="F43" t="inlineStr"/>
-      <c r="G43" t="inlineStr"/>
+      <c r="E43" t="inlineStr">
+        <is>
+          <t>Higher Current rating, Higher insulation resistance, Better resistance to surge current, Low dielectric losses, Long service life, Higher short circuit rating</t>
+        </is>
+      </c>
+      <c r="F43" t="inlineStr">
+        <is>
+          <t>Single core Aluminium, XLPE Insulation , Al round/flat armoured , PVC Outer sheathed cable</t>
+        </is>
+      </c>
+      <c r="G43" t="inlineStr">
+        <is>
+          <t>POLYCAB A2XWaY/A2XFaY SC, stranded compacted aluminium conductor, XLPE insulated, and PVC sheathed armoured cable confirming to IS 7098-1 is suitable for AC single phase or three phase (earthed or unearthed) systems with rated voltage up to and including 1100 V. This cable is also suitable for DC systems with rated voltage up to and including 1500 V</t>
+        </is>
+      </c>
       <c r="H43" t="inlineStr">
         <is>
-          <t>https://polycab.com/polycab-lv-is-7098-i-35c-a2xy/pt-13191/p-54746</t>
-        </is>
-      </c>
-      <c r="I43" t="inlineStr"/>
+          <t>https://polycab.com/polycab-lv-is-7098-i-1c-a2xfay-a2xway/pt-13191/p-54734</t>
+        </is>
+      </c>
+      <c r="I43" t="inlineStr">
+        <is>
+          <t>polycab_lv_power_cable/images/Polycab_LV_IS-7098-I_1C-A2XFaY-A2XWaY_image.png</t>
+        </is>
+      </c>
       <c r="J43" t="inlineStr">
         <is>
-          <t>polycab_lv_power_cable/brochures/Polycab_LV_IS-7098-I_35C-A2XY_datasheet.pdf</t>
+          <t>polycab_lv_power_cable/brochures/Polycab_LV_IS-7098-I_1C-A2XFaY-A2XWaY_datasheet.pdf</t>
         </is>
       </c>
       <c r="K43" t="inlineStr">
         <is>
-          <t>Not Found</t>
+          <t>Downloaded</t>
         </is>
       </c>
       <c r="L43" t="inlineStr">
@@ -2544,7 +3116,7 @@
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t>Polycab BS 5467 MC 0.6/1kV AC</t>
+          <t>Polycab LV IS-7098-I 3C-A2XY</t>
         </is>
       </c>
       <c r="B44" t="inlineStr">
@@ -2554,35 +3126,47 @@
       </c>
       <c r="C44" t="inlineStr">
         <is>
-          <t>IEC 60502-1, BS 5467</t>
+          <t>IS 7098-I</t>
         </is>
       </c>
       <c r="D44" t="inlineStr">
         <is>
-          <t>CE, FQC</t>
+          <t>CE, BIS, CPRI, FQC</t>
         </is>
       </c>
       <c r="E44" t="inlineStr">
         <is>
-          <t>High Life, Low Smoke</t>
-        </is>
-      </c>
-      <c r="F44" t="inlineStr"/>
-      <c r="G44" t="inlineStr"/>
+          <t>Higher insulation resistance, Better resistance to surge currents, Low dielectric losses, Long service life, Higher short circuit rating</t>
+        </is>
+      </c>
+      <c r="F44" t="inlineStr">
+        <is>
+          <t>Three core Aluminium, XLPE Insulation, PVC inner sheathed, unarmoured, PVC Outer sheathed cable</t>
+        </is>
+      </c>
+      <c r="G44" t="inlineStr">
+        <is>
+          <t>POLYCAB A2XY MC-3, Stranded compacted aluminium conductor, XLPE insulated, and PVC sheathed confirming to IS 7098-1 is suitable for AC single phase or three phase (earthed or unearthed) systems with rated voltage up to and including 1100 V. This cable is also suitable for DC systems with rated voltage up to and including 1500 V</t>
+        </is>
+      </c>
       <c r="H44" t="inlineStr">
         <is>
-          <t>https://polycab.com/polycab-bs-5467-mc-061kv-ac/pt-13191/p-55467</t>
-        </is>
-      </c>
-      <c r="I44" t="inlineStr"/>
+          <t>https://polycab.com/polycab-lv-is-7098-i-3c-a2xy/pt-13191/p-54750</t>
+        </is>
+      </c>
+      <c r="I44" t="inlineStr">
+        <is>
+          <t>polycab_lv_power_cable/images/Polycab_LV_IS-7098-I_3C-A2XY_image.png</t>
+        </is>
+      </c>
       <c r="J44" t="inlineStr">
         <is>
-          <t>polycab_lv_power_cable/brochures/Polycab_BS_5467_MC_061kV_AC_datasheet.pdf</t>
+          <t>polycab_lv_power_cable/brochures/Polycab_LV_IS-7098-I_3C-A2XY_datasheet.pdf</t>
         </is>
       </c>
       <c r="K44" t="inlineStr">
         <is>
-          <t>Not Found</t>
+          <t>Downloaded</t>
         </is>
       </c>
       <c r="L44" t="inlineStr">
@@ -2594,7 +3178,7 @@
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
-          <t>Polycab LV IS-7098-I 4C A2XWY</t>
+          <t>Polycab LV Cu IEC 60502-1 0.6/1kV MC-2 UA</t>
         </is>
       </c>
       <c r="B45" t="inlineStr">
@@ -2604,31 +3188,47 @@
       </c>
       <c r="C45" t="inlineStr">
         <is>
-          <t>IEC 60502-1, IS 7098-1, BS 5467</t>
+          <t>IEC 60502-1</t>
         </is>
       </c>
       <c r="D45" t="inlineStr">
         <is>
-          <t>CE, BIS, CPRI, FQC</t>
-        </is>
-      </c>
-      <c r="E45" t="inlineStr"/>
-      <c r="F45" t="inlineStr"/>
-      <c r="G45" t="inlineStr"/>
+          <t>CE, FQC</t>
+        </is>
+      </c>
+      <c r="E45" t="inlineStr">
+        <is>
+          <t>Higher dielectric strength, Better electrical, mechanical, And thermal properties, UV resistant, Long service life, Low smoke emission</t>
+        </is>
+      </c>
+      <c r="F45" t="inlineStr">
+        <is>
+          <t>Multi core stranded copper conductor, XLPE/EPR/HEPR insulation, Laid up, Inner covering, Armoured, PVC/Polyethylene/Halogen free Outer sheathed LV Cable</t>
+        </is>
+      </c>
+      <c r="G45" t="inlineStr">
+        <is>
+          <t>Multicore stranded Copper, XLPE/EPR/HEPR insulation, Laid up, inner covering,PVC/Polyethylene/Halogen free sheathed unarmored Cable suitable for fixed installation such as distribution network or industrial installation.These cables are designed for systems with rated AC voltage 1KV (Um=1.2 KV) between two live conductor.</t>
+        </is>
+      </c>
       <c r="H45" t="inlineStr">
         <is>
-          <t>https://polycab.com/polycab-lv-is-7098-i-4c-a2xwy/pt-13191/p-54730</t>
-        </is>
-      </c>
-      <c r="I45" t="inlineStr"/>
+          <t>https://polycab.com/polycab-lv-cu-iec-60502-1-061kv-mc-2-ua/pt-13191/p-55265</t>
+        </is>
+      </c>
+      <c r="I45" t="inlineStr">
+        <is>
+          <t>polycab_lv_power_cable/images/Polycab_LV_Cu_IEC_60502-1_061kV_MC-2_UA_image.png</t>
+        </is>
+      </c>
       <c r="J45" t="inlineStr">
         <is>
-          <t>polycab_lv_power_cable/brochures/Polycab_LV_IS-7098-I_4C_A2XWY_datasheet.pdf</t>
+          <t>polycab_lv_power_cable/brochures/Polycab_LV_Cu_IEC_60502-1_061kV_MC-2_UA_datasheet.pdf</t>
         </is>
       </c>
       <c r="K45" t="inlineStr">
         <is>
-          <t>Not Found</t>
+          <t>Downloaded</t>
         </is>
       </c>
       <c r="L45" t="inlineStr">
@@ -2640,7 +3240,7 @@
     <row r="46">
       <c r="A46" t="inlineStr">
         <is>
-          <t>Polycab LV Cu IEC 60502-1 0.6/1kV MC-2 UA</t>
+          <t>Polycab LV Cu IEC 60502-1 0.6/1kV MC-3 SFA</t>
         </is>
       </c>
       <c r="B46" t="inlineStr">
@@ -2650,7 +3250,7 @@
       </c>
       <c r="C46" t="inlineStr">
         <is>
-          <t>IEC 60502-1, BS 5467</t>
+          <t>IEC 60502-1</t>
         </is>
       </c>
       <c r="D46" t="inlineStr">
@@ -2660,25 +3260,37 @@
       </c>
       <c r="E46" t="inlineStr">
         <is>
-          <t>UV Resistant, Low Smoke</t>
-        </is>
-      </c>
-      <c r="F46" t="inlineStr"/>
-      <c r="G46" t="inlineStr"/>
+          <t>Higher dielectric strength, Better electrical, mechanical, And thermal properties, UV resistant, Long service life, Low smoke emission</t>
+        </is>
+      </c>
+      <c r="F46" t="inlineStr">
+        <is>
+          <t>Multi core stranded copper conductor,XLPE/EPR/HEPR insulation, Laid up, Inner covering, Armoured, PVC/Polyethylene/Halogen free Outer sheathed LV Cable</t>
+        </is>
+      </c>
+      <c r="G46" t="inlineStr">
+        <is>
+          <t>Multicore stranded Copper conductor, XLPE/EPR/HEPR insulation, Laid up, inner covering,GI flat strip armoured,PVC/Polyethylene/Halogen free sheathed. suitable for fixed installation such as distribution network or industrial installation. These cable cables are designed for systems with rated AC voltage 1KV (Um=1.2 KV) between two live conductor.</t>
+        </is>
+      </c>
       <c r="H46" t="inlineStr">
         <is>
-          <t>https://polycab.com/polycab-lv-cu-iec-60502-1-061kv-mc-2-ua/pt-13191/p-55265</t>
-        </is>
-      </c>
-      <c r="I46" t="inlineStr"/>
+          <t>https://polycab.com/polycab-lv-cu-iec-60502-1-061kv-mc-3-sfa/pt-13191/p-55285</t>
+        </is>
+      </c>
+      <c r="I46" t="inlineStr">
+        <is>
+          <t>polycab_lv_power_cable/images/Polycab_LV_Cu_IEC_60502-1_061kV_MC-3_SFA_image.png</t>
+        </is>
+      </c>
       <c r="J46" t="inlineStr">
         <is>
-          <t>polycab_lv_power_cable/brochures/Polycab_LV_Cu_IEC_60502-1_061kV_MC-2_UA_datasheet.pdf</t>
+          <t>polycab_lv_power_cable/brochures/Polycab_LV_Cu_IEC_60502-1_061kV_MC-3_SFA_datasheet.pdf</t>
         </is>
       </c>
       <c r="K46" t="inlineStr">
         <is>
-          <t>Not Found</t>
+          <t>Downloaded</t>
         </is>
       </c>
       <c r="L46" t="inlineStr">
@@ -2690,7 +3302,7 @@
     <row r="47">
       <c r="A47" t="inlineStr">
         <is>
-          <t>Polycab LV IS-7098-I 2C-A2XY</t>
+          <t>Polycab BS 5467 MC 0.6/1kV AC</t>
         </is>
       </c>
       <c r="B47" t="inlineStr">
@@ -2700,31 +3312,47 @@
       </c>
       <c r="C47" t="inlineStr">
         <is>
-          <t>IEC 60502-1, IS 7098-1, BS 5467</t>
+          <t>BS 5467</t>
         </is>
       </c>
       <c r="D47" t="inlineStr">
         <is>
-          <t>CE, BIS, CPRI, FQC</t>
-        </is>
-      </c>
-      <c r="E47" t="inlineStr"/>
-      <c r="F47" t="inlineStr"/>
-      <c r="G47" t="inlineStr"/>
+          <t>CE, FQC</t>
+        </is>
+      </c>
+      <c r="E47" t="inlineStr">
+        <is>
+          <t>Low flame propagation, Low smoke emission, High life, Resistant to weather exposure</t>
+        </is>
+      </c>
+      <c r="F47" t="inlineStr">
+        <is>
+          <t>Stranded copper conductor, XLPE/EPR Insulated, Extruded Polymeric Bedding, GS round wire armoured,PVC FRLS Outer Sheathed 0.6/1 kV LV Cable</t>
+        </is>
+      </c>
+      <c r="G47" t="inlineStr">
+        <is>
+          <t>POLYCAB BS 5467 MC stranded copper conductor thermosetting material insulated Multi core armoured cable fulfils the requirement as per BS EN 5467. These cables are suitable for fixed installation in industrial area, buildings, Power network in underground, outdoor, indoor and similar application where mechanical protection is required.</t>
+        </is>
+      </c>
       <c r="H47" t="inlineStr">
         <is>
-          <t>https://polycab.com/polycab-lv-is-7098-i-2c-a2xy/pt-13191/p-54742</t>
-        </is>
-      </c>
-      <c r="I47" t="inlineStr"/>
+          <t>https://polycab.com/polycab-bs-5467-mc-061kv-ac/pt-13191/p-55467</t>
+        </is>
+      </c>
+      <c r="I47" t="inlineStr">
+        <is>
+          <t>polycab_lv_power_cable/images/Polycab_BS_5467_MC_061kV_AC_image.png</t>
+        </is>
+      </c>
       <c r="J47" t="inlineStr">
         <is>
-          <t>polycab_lv_power_cable/brochures/Polycab_LV_IS-7098-I_2C-A2XY_datasheet.pdf</t>
+          <t>polycab_lv_power_cable/brochures/Polycab_BS_5467_MC_061kV_AC_datasheet.pdf</t>
         </is>
       </c>
       <c r="K47" t="inlineStr">
         <is>
-          <t>Not Found</t>
+          <t>Downloaded</t>
         </is>
       </c>
       <c r="L47" t="inlineStr">
@@ -2736,7 +3364,7 @@
     <row r="48">
       <c r="A48" t="inlineStr">
         <is>
-          <t>Polycab LV Cu IEC 60502-1 0.6/1kV MC-3.5 UA</t>
+          <t>Polycab LV IS-7098-I 1C-2XFaY-2XWaY</t>
         </is>
       </c>
       <c r="B48" t="inlineStr">
@@ -2746,35 +3374,47 @@
       </c>
       <c r="C48" t="inlineStr">
         <is>
-          <t>IEC 60502-1, BS 5467</t>
+          <t>IS 7098-I</t>
         </is>
       </c>
       <c r="D48" t="inlineStr">
         <is>
-          <t>CE, FQC</t>
+          <t>CE, BIS, CPRI, FQC</t>
         </is>
       </c>
       <c r="E48" t="inlineStr">
         <is>
-          <t>UV Resistant, Low Smoke</t>
-        </is>
-      </c>
-      <c r="F48" t="inlineStr"/>
-      <c r="G48" t="inlineStr"/>
+          <t>Higher Current rating, Higher insulation resistance, Better resistance to surge current, Low dielectric losses, Long service life, Higher short circuit rating</t>
+        </is>
+      </c>
+      <c r="F48" t="inlineStr">
+        <is>
+          <t>Single core Aluminium, XLPE Insulation ,Al round/flat armoured , PVC Outer sheathed cable</t>
+        </is>
+      </c>
+      <c r="G48" t="inlineStr">
+        <is>
+          <t>POLYCAB 2XWaY/2XFaY SC, stranded compacted copper conductor, XLPE insulated and PVC sheathed armoured cable confirming to IS 7098-1 is suitable for AC single phase or three phase (earthed or unearthed) systems with rated voltage up to and including 1100 V. This cable is also suitable for DC systems with rated voltage up to and including 1500 V</t>
+        </is>
+      </c>
       <c r="H48" t="inlineStr">
         <is>
-          <t>https://polycab.com/polycab-lv-cu-iec-60502-1-061kv-mc-35-ua/pt-13191/p-55277</t>
-        </is>
-      </c>
-      <c r="I48" t="inlineStr"/>
+          <t>https://polycab.com/polycab-lv-is-7098-i-1c-2xfay-2xway/pt-13191/p-54732</t>
+        </is>
+      </c>
+      <c r="I48" t="inlineStr">
+        <is>
+          <t>polycab_lv_power_cable/images/Polycab_LV_IS-7098-I_1C-2XFaY-2XWaY_image.png</t>
+        </is>
+      </c>
       <c r="J48" t="inlineStr">
         <is>
-          <t>polycab_lv_power_cable/brochures/Polycab_LV_Cu_IEC_60502-1_061kV_MC-35_UA_datasheet.pdf</t>
+          <t>polycab_lv_power_cable/brochures/Polycab_LV_IS-7098-I_1C-2XFaY-2XWaY_datasheet.pdf</t>
         </is>
       </c>
       <c r="K48" t="inlineStr">
         <is>
-          <t>Not Found</t>
+          <t>Downloaded</t>
         </is>
       </c>
       <c r="L48" t="inlineStr">
@@ -2786,7 +3426,7 @@
     <row r="49">
       <c r="A49" t="inlineStr">
         <is>
-          <t>Polycab LV AL IEC 60502-1 0.6/1kV SC AWA</t>
+          <t>Polycab LV IS-7098-I 4C A2XWY</t>
         </is>
       </c>
       <c r="B49" t="inlineStr">
@@ -2796,35 +3436,47 @@
       </c>
       <c r="C49" t="inlineStr">
         <is>
-          <t>IEC 60502-1, BS 5467</t>
+          <t>IS 7098-I</t>
         </is>
       </c>
       <c r="D49" t="inlineStr">
         <is>
-          <t>CE, FQC</t>
+          <t>CE, BIS, CPRI, FQC</t>
         </is>
       </c>
       <c r="E49" t="inlineStr">
         <is>
-          <t>UV Resistant, Low Smoke</t>
-        </is>
-      </c>
-      <c r="F49" t="inlineStr"/>
-      <c r="G49" t="inlineStr"/>
+          <t>Higher Current rating, Higher insulation resistance, Better resistance to surge current, Low dielectric losses, Long service life, Higher short circuit rating</t>
+        </is>
+      </c>
+      <c r="F49" t="inlineStr">
+        <is>
+          <t>Four core Aluminium, XLPE Insulation, Inner sheathed &amp; GI round armoured &amp; PVC Outer sheathed cable</t>
+        </is>
+      </c>
+      <c r="G49" t="inlineStr">
+        <is>
+          <t>POLYCAB A2XWY MC-4, Stranded compacted aluminium conductor, XLPE insulated, PVC inner sheathed, Galvanised Steel round wire armour and PVC sheathed confirming to IS 7098-1 is suitable for AC single phase or three phase (earthed or unearthed) systems with rated voltage up to and including 1100 V. This cable is also suitable for DC systems with rated voltage up to and including 1500 V</t>
+        </is>
+      </c>
       <c r="H49" t="inlineStr">
         <is>
-          <t>https://polycab.com/polycab-lv-al-iec-60502-1-061kv-sc-awa/pt-13191/p-55245</t>
-        </is>
-      </c>
-      <c r="I49" t="inlineStr"/>
+          <t>https://polycab.com/polycab-lv-is-7098-i-4c-a2xwy/pt-13191/p-54730</t>
+        </is>
+      </c>
+      <c r="I49" t="inlineStr">
+        <is>
+          <t>polycab_lv_power_cable/images/Polycab_LV_IS-7098-I_4C_A2XWY_image.png</t>
+        </is>
+      </c>
       <c r="J49" t="inlineStr">
         <is>
-          <t>polycab_lv_power_cable/brochures/Polycab_LV_AL_IEC_60502-1_061kV_SC_AWA_datasheet.pdf</t>
+          <t>polycab_lv_power_cable/brochures/Polycab_LV_IS-7098-I_4C_A2XWY_datasheet.pdf</t>
         </is>
       </c>
       <c r="K49" t="inlineStr">
         <is>
-          <t>Not Found</t>
+          <t>Downloaded</t>
         </is>
       </c>
       <c r="L49" t="inlineStr">
@@ -2836,7 +3488,7 @@
     <row r="50">
       <c r="A50" t="inlineStr">
         <is>
-          <t>Polycab LV Cu IEC 60502-1 0.6/1kV MC-2 SWA</t>
+          <t>Polycab LV IS-7098-I 2C-A2XY</t>
         </is>
       </c>
       <c r="B50" t="inlineStr">
@@ -2846,35 +3498,47 @@
       </c>
       <c r="C50" t="inlineStr">
         <is>
-          <t>IEC 60502-1, BS 5467</t>
+          <t>IS 7098-I</t>
         </is>
       </c>
       <c r="D50" t="inlineStr">
         <is>
-          <t>CE, FQC</t>
+          <t>CE, BIS, CPRI, FQC</t>
         </is>
       </c>
       <c r="E50" t="inlineStr">
         <is>
-          <t>UV Resistant, Low Smoke</t>
-        </is>
-      </c>
-      <c r="F50" t="inlineStr"/>
-      <c r="G50" t="inlineStr"/>
+          <t>Higher insulation resistance, Better resistance to surge currents, Low dielectric losses, Long service life, Higher short circuit rating</t>
+        </is>
+      </c>
+      <c r="F50" t="inlineStr">
+        <is>
+          <t>Two core aluminium, XLPE Insulation, PVC inner sheathed, unarmoured ,PVC Outer sheathed cable</t>
+        </is>
+      </c>
+      <c r="G50" t="inlineStr">
+        <is>
+          <t>POLYCAB A2XY MC-2, Stranded compacted aluminium conductor, XLPE insulated and PVC sheathed confirming to IS 7098-1 is suitable for AC single phase or three phase (earthed or unearthed) systems with rated voltage up to and including 1100 V. This cable is also suitable for DC systems with rated voltage up to and including 1500 V</t>
+        </is>
+      </c>
       <c r="H50" t="inlineStr">
         <is>
-          <t>https://polycab.com/polycab-lv-cu-iec-60502-1-061kv-mc-2-swa/pt-13191/p-55263</t>
-        </is>
-      </c>
-      <c r="I50" t="inlineStr"/>
+          <t>https://polycab.com/polycab-lv-is-7098-i-2c-a2xy/pt-13191/p-54742</t>
+        </is>
+      </c>
+      <c r="I50" t="inlineStr">
+        <is>
+          <t>polycab_lv_power_cable/images/Polycab_LV_IS-7098-I_2C-A2XY_image.png</t>
+        </is>
+      </c>
       <c r="J50" t="inlineStr">
         <is>
-          <t>polycab_lv_power_cable/brochures/Polycab_LV_Cu_IEC_60502-1_061kV_MC-2_SWA_datasheet.pdf</t>
+          <t>polycab_lv_power_cable/brochures/Polycab_LV_IS-7098-I_2C-A2XY_datasheet.pdf</t>
         </is>
       </c>
       <c r="K50" t="inlineStr">
         <is>
-          <t>Not Found</t>
+          <t>Downloaded</t>
         </is>
       </c>
       <c r="L50" t="inlineStr">
@@ -2886,7 +3550,7 @@
     <row r="51">
       <c r="A51" t="inlineStr">
         <is>
-          <t>Polycab LV Cu IEC 60502-1 0.6/1kV MC-2 SFA</t>
+          <t>Polycab LV IS-7098-I 3.5C 2XFY</t>
         </is>
       </c>
       <c r="B51" t="inlineStr">
@@ -2896,35 +3560,47 @@
       </c>
       <c r="C51" t="inlineStr">
         <is>
-          <t>IEC 60502-1, BS 5467</t>
+          <t>IS 7098-I</t>
         </is>
       </c>
       <c r="D51" t="inlineStr">
         <is>
-          <t>CE, FQC</t>
+          <t>CE, BIS, CPRI, FQC</t>
         </is>
       </c>
       <c r="E51" t="inlineStr">
         <is>
-          <t>UV Resistant, Low Smoke</t>
-        </is>
-      </c>
-      <c r="F51" t="inlineStr"/>
-      <c r="G51" t="inlineStr"/>
+          <t>Higher Current rating, Higher insulation resistance, Better resistance to surge current, Low dielectric losses, Long service life, Higher short circuit rating</t>
+        </is>
+      </c>
+      <c r="F51" t="inlineStr">
+        <is>
+          <t>Three and half core Copper conductor, XLPE Insulation Inner sheathed &amp; GI flat armoured &amp; PVC Outer sheathed cable</t>
+        </is>
+      </c>
+      <c r="G51" t="inlineStr">
+        <is>
+          <t>POLYCAB 2XFY MC-3.5, Stranded compacted copper conductor, XLPE insulated, PVC inner sheathed, Galvanised Steel Flat strip armour and PVC sheathed confirming to IS 7098-1 is suitable for AC single phase or three phase (earthed or unearthed) systems with rated voltage up to and including 1100 V. This cable is also suitable for DC systems with rated voltage up to and including 1500 V</t>
+        </is>
+      </c>
       <c r="H51" t="inlineStr">
         <is>
-          <t>https://polycab.com/polycab-lv-cu-iec-60502-1-061kv-mc-2-sfa/pt-13191/p-55261</t>
-        </is>
-      </c>
-      <c r="I51" t="inlineStr"/>
+          <t>https://polycab.com/polycab-lv-is-7098-i-35c-2xfy/pt-13191/p-54708</t>
+        </is>
+      </c>
+      <c r="I51" t="inlineStr">
+        <is>
+          <t>polycab_lv_power_cable/images/Polycab_LV_IS-7098-I_35C_2XFY_image.png</t>
+        </is>
+      </c>
       <c r="J51" t="inlineStr">
         <is>
-          <t>polycab_lv_power_cable/brochures/Polycab_LV_Cu_IEC_60502-1_061kV_MC-2_SFA_datasheet.pdf</t>
+          <t>polycab_lv_power_cable/brochures/Polycab_LV_IS-7098-I_35C_2XFY_datasheet.pdf</t>
         </is>
       </c>
       <c r="K51" t="inlineStr">
         <is>
-          <t>Not Found</t>
+          <t>Downloaded</t>
         </is>
       </c>
       <c r="L51" t="inlineStr">
@@ -2936,7 +3612,7 @@
     <row r="52">
       <c r="A52" t="inlineStr">
         <is>
-          <t>Polycab LV IS-7098-I 2C A2XFY</t>
+          <t>Polycab LV IS-7098-I 2C 2XWY</t>
         </is>
       </c>
       <c r="B52" t="inlineStr">
@@ -2946,7 +3622,7 @@
       </c>
       <c r="C52" t="inlineStr">
         <is>
-          <t>IEC 60502-1, IS 7098-1, BS 5467</t>
+          <t>IS 7098-I</t>
         </is>
       </c>
       <c r="D52" t="inlineStr">
@@ -2954,23 +3630,39 @@
           <t>CE, BIS, CPRI, FQC</t>
         </is>
       </c>
-      <c r="E52" t="inlineStr"/>
-      <c r="F52" t="inlineStr"/>
-      <c r="G52" t="inlineStr"/>
+      <c r="E52" t="inlineStr">
+        <is>
+          <t>Higher Current rating, Higher insulation resistance, Better resistance to surge current, Low dielectric losses, Long service life, Higher short circuit rating</t>
+        </is>
+      </c>
+      <c r="F52" t="inlineStr">
+        <is>
+          <t>Two core copper conductor, XLPE Insulation,PVC Inner sheathed &amp; GI round armoured &amp; PVC Outer sheathed cable</t>
+        </is>
+      </c>
+      <c r="G52" t="inlineStr">
+        <is>
+          <t>POLYCAB 2XWY MC-2, stranded compacted copper conductor XLPE insulated, PVC inner sheathed, Galvanised Steel round wire armour and PVC sheathed confirming to IS 7098-1 is suitable for AC single phase or three phase (earthed or unearthed) systems with rated voltage up to and including 1100 V. This cable is also suitable for DC systems with rated voltage up to and including 1500 V</t>
+        </is>
+      </c>
       <c r="H52" t="inlineStr">
         <is>
-          <t>https://polycab.com/polycab-lv-is-7098-i-2c-a2xfy/pt-13191/p-54704</t>
-        </is>
-      </c>
-      <c r="I52" t="inlineStr"/>
+          <t>https://polycab.com/polycab-lv-is-7098-i-2c-2xwy/pt-13191/p-54702</t>
+        </is>
+      </c>
+      <c r="I52" t="inlineStr">
+        <is>
+          <t>polycab_lv_power_cable/images/Polycab_LV_IS-7098-I_2C_2XWY_image.png</t>
+        </is>
+      </c>
       <c r="J52" t="inlineStr">
         <is>
-          <t>polycab_lv_power_cable/brochures/Polycab_LV_IS-7098-I_2C_A2XFY_datasheet.pdf</t>
+          <t>polycab_lv_power_cable/brochures/Polycab_LV_IS-7098-I_2C_2XWY_datasheet.pdf</t>
         </is>
       </c>
       <c r="K52" t="inlineStr">
         <is>
-          <t>Not Found</t>
+          <t>Downloaded</t>
         </is>
       </c>
       <c r="L52" t="inlineStr">
@@ -2982,7 +3674,7 @@
     <row r="53">
       <c r="A53" t="inlineStr">
         <is>
-          <t>Polycab LV AL IEC 60502-1 0.6/1kV MC-2 SWA</t>
+          <t>Polycab LV Cu IEC 60502-1 0.6/1kV SC AWA</t>
         </is>
       </c>
       <c r="B53" t="inlineStr">
@@ -2992,7 +3684,7 @@
       </c>
       <c r="C53" t="inlineStr">
         <is>
-          <t>IEC 60502-1, BS 5467</t>
+          <t>IEC 60502-1</t>
         </is>
       </c>
       <c r="D53" t="inlineStr">
@@ -3002,25 +3694,37 @@
       </c>
       <c r="E53" t="inlineStr">
         <is>
-          <t>UV Resistant, Low Smoke</t>
-        </is>
-      </c>
-      <c r="F53" t="inlineStr"/>
-      <c r="G53" t="inlineStr"/>
+          <t>Higher dielectric strength, Better electrical, mechanical, And thermal properties, UV resistant, Long service life, Low smoke emission</t>
+        </is>
+      </c>
+      <c r="F53" t="inlineStr">
+        <is>
+          <t>Single core stranded Copper conductor,XLPE/EPR/HEPR insulation, Aluminium wire armoured,PVC/Polyethylene/Halogen free Outer sheathed LV Cable</t>
+        </is>
+      </c>
+      <c r="G53" t="inlineStr">
+        <is>
+          <t>Single core stranded copper conductor, XLPE/EPR/HEPR insulation,PVC/Polyethylene/Halogen free Inner, Aluminium wire armored &amp; outer sheathed Cable. suitable for fixed installation such as distribution network or industrial installation. These cable cables are designed for systems with rated AC voltage 1KV (Um=1.2 KV).</t>
+        </is>
+      </c>
       <c r="H53" t="inlineStr">
         <is>
-          <t>https://polycab.com/polycab-lv-al-iec-60502-1-061kv-mc-2-swa/pt-13191/p-55257</t>
-        </is>
-      </c>
-      <c r="I53" t="inlineStr"/>
+          <t>https://polycab.com/polycab-lv-cu-iec-60502-1-061kv-sc-awa/pt-13191/p-55249</t>
+        </is>
+      </c>
+      <c r="I53" t="inlineStr">
+        <is>
+          <t>polycab_lv_power_cable/images/Polycab_LV_Cu_IEC_60502-1_061kV_SC_AWA_image.png</t>
+        </is>
+      </c>
       <c r="J53" t="inlineStr">
         <is>
-          <t>polycab_lv_power_cable/brochures/Polycab_LV_AL_IEC_60502-1_061kV_MC-2_SWA_datasheet.pdf</t>
+          <t>polycab_lv_power_cable/brochures/Polycab_LV_Cu_IEC_60502-1_061kV_SC_AWA_datasheet.pdf</t>
         </is>
       </c>
       <c r="K53" t="inlineStr">
         <is>
-          <t>Not Found</t>
+          <t>Downloaded</t>
         </is>
       </c>
       <c r="L53" t="inlineStr">
@@ -3032,7 +3736,7 @@
     <row r="54">
       <c r="A54" t="inlineStr">
         <is>
-          <t>Polycab LV Cu IEC 60502-1 0.6/1kV SC SFA</t>
+          <t>Polycab LV IS-7098-I 3C 2XWY</t>
         </is>
       </c>
       <c r="B54" t="inlineStr">
@@ -3042,35 +3746,47 @@
       </c>
       <c r="C54" t="inlineStr">
         <is>
-          <t>IEC 60502-1, BS 5467</t>
+          <t>IS 7098-I</t>
         </is>
       </c>
       <c r="D54" t="inlineStr">
         <is>
-          <t>CE, FQC</t>
+          <t>CE, BIS, CPRI, FQC</t>
         </is>
       </c>
       <c r="E54" t="inlineStr">
         <is>
-          <t>UV Resistant, Low Smoke</t>
-        </is>
-      </c>
-      <c r="F54" t="inlineStr"/>
-      <c r="G54" t="inlineStr"/>
+          <t>Higher Current rating, Higher insulation resistance, Better resistance to surge current, Low dielectric losses, Long service life, Higher short circuit rating</t>
+        </is>
+      </c>
+      <c r="F54" t="inlineStr">
+        <is>
+          <t>Three core copper conductor, XLPE Insulation, Inner sheathed &amp; GI round armoured &amp; PVC Outer sheathed cable</t>
+        </is>
+      </c>
+      <c r="G54" t="inlineStr">
+        <is>
+          <t>POLYCAB 2XWY MC-3, Stranded compacted copper conductor, XLPE insulated, PVC inner sheathed, Galvanised Steel round wire armour and PVC sheathed confirming to IS 7098-1 is suitable for AC single phase or three phase (earthed or unearthed) systems with rated voltage up to and including 1100 V. This cable is also suitable for DC systems with rated voltage up to and including 1500 V</t>
+        </is>
+      </c>
       <c r="H54" t="inlineStr">
         <is>
-          <t>https://polycab.com/polycab-lv-cu-iec-60502-1-061kv-sc-sfa/pt-13191/p-55251</t>
-        </is>
-      </c>
-      <c r="I54" t="inlineStr"/>
+          <t>https://polycab.com/polycab-lv-is-7098-i-3c-2xwy/pt-13191/p-54718</t>
+        </is>
+      </c>
+      <c r="I54" t="inlineStr">
+        <is>
+          <t>polycab_lv_power_cable/images/Polycab_LV_IS-7098-I_3C_2XWY_image.png</t>
+        </is>
+      </c>
       <c r="J54" t="inlineStr">
         <is>
-          <t>polycab_lv_power_cable/brochures/Polycab_LV_Cu_IEC_60502-1_061kV_SC_SFA_datasheet.pdf</t>
+          <t>polycab_lv_power_cable/brochures/Polycab_LV_IS-7098-I_3C_2XWY_datasheet.pdf</t>
         </is>
       </c>
       <c r="K54" t="inlineStr">
         <is>
-          <t>Not Found</t>
+          <t>Downloaded</t>
         </is>
       </c>
       <c r="L54" t="inlineStr">
@@ -3082,7 +3798,7 @@
     <row r="55">
       <c r="A55" t="inlineStr">
         <is>
-          <t>Polycab LV Cu IEC 60502-1 0.6/1kV MC-3 SWA</t>
+          <t>Polycab LV IS-7098-I 4C-2XY</t>
         </is>
       </c>
       <c r="B55" t="inlineStr">
@@ -3092,35 +3808,47 @@
       </c>
       <c r="C55" t="inlineStr">
         <is>
-          <t>IEC 60502-1, BS 5467</t>
+          <t>IS 7098-I</t>
         </is>
       </c>
       <c r="D55" t="inlineStr">
         <is>
-          <t>CE, FQC</t>
+          <t>CE, BIS, CPRI, FQC</t>
         </is>
       </c>
       <c r="E55" t="inlineStr">
         <is>
-          <t>UV Resistant, Low Smoke</t>
-        </is>
-      </c>
-      <c r="F55" t="inlineStr"/>
-      <c r="G55" t="inlineStr"/>
+          <t>Higher insulation resistance, Better resistance to surge currents, Low dielectric losses, Long service life, Higher short circuit rating</t>
+        </is>
+      </c>
+      <c r="F55" t="inlineStr">
+        <is>
+          <t>Four core copper, XLPE Insulation, PVC inner sheathed, unarmoured, PVC Outer sheathed cable</t>
+        </is>
+      </c>
+      <c r="G55" t="inlineStr">
+        <is>
+          <t>POLYCAB 2XY MC-4, Stranded compacted copper conductor, XLPE insulated, and PVC sheathed confirming to IS 7098-1 is suitable for AC single phase or three phase (earthed or unearthed) systems with rated voltage up to and including 1100 V. This cable is also suitable for DC systems with rated voltage up to and including 1500 V</t>
+        </is>
+      </c>
       <c r="H55" t="inlineStr">
         <is>
-          <t>https://polycab.com/polycab-lv-cu-iec-60502-1-061kv-mc-3-swa/pt-13191/p-55287</t>
-        </is>
-      </c>
-      <c r="I55" t="inlineStr"/>
+          <t>https://polycab.com/polycab-lv-is-7098-i-4c-2xy/pt-13191/p-54752</t>
+        </is>
+      </c>
+      <c r="I55" t="inlineStr">
+        <is>
+          <t>polycab_lv_power_cable/images/Polycab_LV_IS-7098-I_4C-2XY_image.png</t>
+        </is>
+      </c>
       <c r="J55" t="inlineStr">
         <is>
-          <t>polycab_lv_power_cable/brochures/Polycab_LV_Cu_IEC_60502-1_061kV_MC-3_SWA_datasheet.pdf</t>
+          <t>polycab_lv_power_cable/brochures/Polycab_LV_IS-7098-I_4C-2XY_datasheet.pdf</t>
         </is>
       </c>
       <c r="K55" t="inlineStr">
         <is>
-          <t>Not Found</t>
+          <t>Downloaded</t>
         </is>
       </c>
       <c r="L55" t="inlineStr">
@@ -3132,7 +3860,7 @@
     <row r="56">
       <c r="A56" t="inlineStr">
         <is>
-          <t>Polycab LV IS-7098-I 4C 2XFY</t>
+          <t>Polycab LV IS-7098-I 2C A2XFY</t>
         </is>
       </c>
       <c r="B56" t="inlineStr">
@@ -3142,7 +3870,7 @@
       </c>
       <c r="C56" t="inlineStr">
         <is>
-          <t>IEC 60502-1, IS 7098-1, BS 5467</t>
+          <t>IS 7098-I</t>
         </is>
       </c>
       <c r="D56" t="inlineStr">
@@ -3150,23 +3878,39 @@
           <t>CE, BIS, CPRI, FQC</t>
         </is>
       </c>
-      <c r="E56" t="inlineStr"/>
-      <c r="F56" t="inlineStr"/>
-      <c r="G56" t="inlineStr"/>
+      <c r="E56" t="inlineStr">
+        <is>
+          <t>Higher Current rating, Higher insulation resistance, Better resistance to surge current, Low dielectric losses, Long service life, Higher short circuit rating</t>
+        </is>
+      </c>
+      <c r="F56" t="inlineStr">
+        <is>
+          <t>Two core Aluminium conductor, XLPE Insulation,PVC Inner sheathed &amp; GI flat armoured &amp; PVC Outer sheathed cable</t>
+        </is>
+      </c>
+      <c r="G56" t="inlineStr">
+        <is>
+          <t>POLYCAB A2XFY MC-2, Stranded compacted aluminium conductor, XLPE insulated, PVC inner sheathed, Galvanised Steel Flat strip armour and PVC sheathed confirming to IS 7098-1 is suitable for AC single phase or three phase (earthed or unearthed) systems with rated voltage up to and including 1100 V. This cable is also suitable for DC systems with rated voltage up to and including 1500 V</t>
+        </is>
+      </c>
       <c r="H56" t="inlineStr">
         <is>
-          <t>https://polycab.com/polycab-lv-is-7098-i-4c-2xfy/pt-13191/p-54724</t>
-        </is>
-      </c>
-      <c r="I56" t="inlineStr"/>
+          <t>https://polycab.com/polycab-lv-is-7098-i-2c-a2xfy/pt-13191/p-54704</t>
+        </is>
+      </c>
+      <c r="I56" t="inlineStr">
+        <is>
+          <t>polycab_lv_power_cable/images/Polycab_LV_IS-7098-I_2C_A2XFY_image.png</t>
+        </is>
+      </c>
       <c r="J56" t="inlineStr">
         <is>
-          <t>polycab_lv_power_cable/brochures/Polycab_LV_IS-7098-I_4C_2XFY_datasheet.pdf</t>
+          <t>polycab_lv_power_cable/brochures/Polycab_LV_IS-7098-I_2C_A2XFY_datasheet.pdf</t>
         </is>
       </c>
       <c r="K56" t="inlineStr">
         <is>
-          <t>Not Found</t>
+          <t>Downloaded</t>
         </is>
       </c>
       <c r="L56" t="inlineStr">
@@ -3178,7 +3922,7 @@
     <row r="57">
       <c r="A57" t="inlineStr">
         <is>
-          <t>Polycab LV IS-7098-I 3C A2XFY</t>
+          <t>Polycab BS 5467 SC 0.6/1kV AC</t>
         </is>
       </c>
       <c r="B57" t="inlineStr">
@@ -3188,31 +3932,47 @@
       </c>
       <c r="C57" t="inlineStr">
         <is>
-          <t>IEC 60502-1, IS 7098-1, BS 5467</t>
+          <t>BS 5467</t>
         </is>
       </c>
       <c r="D57" t="inlineStr">
         <is>
-          <t>CE, BIS, CPRI, FQC</t>
-        </is>
-      </c>
-      <c r="E57" t="inlineStr"/>
-      <c r="F57" t="inlineStr"/>
-      <c r="G57" t="inlineStr"/>
+          <t>CE, FQC</t>
+        </is>
+      </c>
+      <c r="E57" t="inlineStr">
+        <is>
+          <t>Low flame propagation, Low smoke emission, High life, Resistant to weather exposure</t>
+        </is>
+      </c>
+      <c r="F57" t="inlineStr">
+        <is>
+          <t>Stranded copper conductor, XLPE/EPR Insulated, Extruded Polymeric Bedding, Aluminium round wire armoured, PVC FRLS Outer Sheathed 0.6/1 kV LV cable</t>
+        </is>
+      </c>
+      <c r="G57" t="inlineStr">
+        <is>
+          <t>POLYCAB BS 5467 SC stranded copper conductor thermosetting material insulated Multi core armoured cable fulfils the requirement as per BS EN 5467. These cables are suitable for fixed installation in industrial area, buildings, and similar application</t>
+        </is>
+      </c>
       <c r="H57" t="inlineStr">
         <is>
-          <t>https://polycab.com/polycab-lv-is-7098-i-3c-a2xfy/pt-13191/p-54720</t>
-        </is>
-      </c>
-      <c r="I57" t="inlineStr"/>
+          <t>https://polycab.com/polycab-bs-5467-sc-061kv-ac/pt-13191/p-55465</t>
+        </is>
+      </c>
+      <c r="I57" t="inlineStr">
+        <is>
+          <t>polycab_lv_power_cable/images/Polycab_BS_5467_SC_061kV_AC_image.png</t>
+        </is>
+      </c>
       <c r="J57" t="inlineStr">
         <is>
-          <t>polycab_lv_power_cable/brochures/Polycab_LV_IS-7098-I_3C_A2XFY_datasheet.pdf</t>
+          <t>polycab_lv_power_cable/brochures/Polycab_BS_5467_SC_061kV_AC_datasheet.pdf</t>
         </is>
       </c>
       <c r="K57" t="inlineStr">
         <is>
-          <t>Not Found</t>
+          <t>Downloaded</t>
         </is>
       </c>
       <c r="L57" t="inlineStr">
@@ -3224,7 +3984,7 @@
     <row r="58">
       <c r="A58" t="inlineStr">
         <is>
-          <t>Polycab LV IS-7098-I 3C A2XWY</t>
+          <t>Polycab LV Cu IEC 60502-1 0.6/1kV MC-3.5 UA</t>
         </is>
       </c>
       <c r="B58" t="inlineStr">
@@ -3234,31 +3994,47 @@
       </c>
       <c r="C58" t="inlineStr">
         <is>
-          <t>IEC 60502-1, IS 7098-1, BS 5467</t>
+          <t>IEC 60502-1</t>
         </is>
       </c>
       <c r="D58" t="inlineStr">
         <is>
-          <t>CE, BIS, CPRI, FQC</t>
-        </is>
-      </c>
-      <c r="E58" t="inlineStr"/>
-      <c r="F58" t="inlineStr"/>
-      <c r="G58" t="inlineStr"/>
+          <t>CE, FQC</t>
+        </is>
+      </c>
+      <c r="E58" t="inlineStr">
+        <is>
+          <t>Higher dielectric strength, Better electrical, mechanical, And thermal properties, UV resistant, Long service life, Low smoke emission</t>
+        </is>
+      </c>
+      <c r="F58" t="inlineStr">
+        <is>
+          <t>Multi core stranded copper conductor, XLPE/EPR/HEPR insulation, Laid up, Inner covering, Armoured, PVC/Polyethylene/Halogen free Outer sheathed LV Cable</t>
+        </is>
+      </c>
+      <c r="G58" t="inlineStr">
+        <is>
+          <t>Multicore stranded Copper, XLPE/EPR/HEPR insulation, Laid up, inner covering,PVC/Polyethylene/Halogen free sheathed unarmored Cable suitable for fixed installation such as distribution network or industrial installation.These cables are designed for systems with rated AC voltage 1KV (Um=1.2 KV) between two live conductor.</t>
+        </is>
+      </c>
       <c r="H58" t="inlineStr">
         <is>
-          <t>https://polycab.com/polycab-lv-is-7098-i-3c-a2xwy/pt-13191/p-54722</t>
-        </is>
-      </c>
-      <c r="I58" t="inlineStr"/>
+          <t>https://polycab.com/polycab-lv-cu-iec-60502-1-061kv-mc-35-ua/pt-13191/p-55277</t>
+        </is>
+      </c>
+      <c r="I58" t="inlineStr">
+        <is>
+          <t>polycab_lv_power_cable/images/Polycab_LV_Cu_IEC_60502-1_061kV_MC-35_UA_image.png</t>
+        </is>
+      </c>
       <c r="J58" t="inlineStr">
         <is>
-          <t>polycab_lv_power_cable/brochures/Polycab_LV_IS-7098-I_3C_A2XWY_datasheet.pdf</t>
+          <t>polycab_lv_power_cable/brochures/Polycab_LV_Cu_IEC_60502-1_061kV_MC-35_UA_datasheet.pdf</t>
         </is>
       </c>
       <c r="K58" t="inlineStr">
         <is>
-          <t>Not Found</t>
+          <t>Downloaded</t>
         </is>
       </c>
       <c r="L58" t="inlineStr">
@@ -3270,7 +4046,7 @@
     <row r="59">
       <c r="A59" t="inlineStr">
         <is>
-          <t>Polycab LV AL IEC 60502-1 0.6/1kV MC-4 SFA</t>
+          <t>Polycab LV Cu IEC 60502-1 0.6/1kV MC-4 SFA</t>
         </is>
       </c>
       <c r="B59" t="inlineStr">
@@ -3280,7 +4056,7 @@
       </c>
       <c r="C59" t="inlineStr">
         <is>
-          <t>IEC 60502-1, BS 5467</t>
+          <t>IEC 60502-1</t>
         </is>
       </c>
       <c r="D59" t="inlineStr">
@@ -3290,25 +4066,37 @@
       </c>
       <c r="E59" t="inlineStr">
         <is>
-          <t>UV Resistant, Low Smoke</t>
-        </is>
-      </c>
-      <c r="F59" t="inlineStr"/>
-      <c r="G59" t="inlineStr"/>
+          <t>Higher dielectric strength, Better electrical, mechanical, And thermal properties, UV resistant, Long service life, Low smoke emission</t>
+        </is>
+      </c>
+      <c r="F59" t="inlineStr">
+        <is>
+          <t>Multi core stranded copper conductor, XLPE/EPR/HEPR insulation, Laid up, Inner covering, Armoured, PVC/Polyethylene/Halogen free i Outer sheathed LV Cable</t>
+        </is>
+      </c>
+      <c r="G59" t="inlineStr">
+        <is>
+          <t>Multicore stranded Copper conductor, XLPE/EPR/HEPR insulation, Laid up, inner covering,GI flat strip armoured,PVC/Polyethylene/Halogen free sheathed. suitable for fixed installation such as distribution network or industrial installation. These cable cables are designed for systems with rated AC voltage 1KV (Um=1.2 KV) between two live conductor.</t>
+        </is>
+      </c>
       <c r="H59" t="inlineStr">
         <is>
-          <t>https://polycab.com/polycab-lv-al-iec-60502-1-061kv-mc-4-sfa/pt-13191/p-55291</t>
-        </is>
-      </c>
-      <c r="I59" t="inlineStr"/>
+          <t>https://polycab.com/polycab-lv-cu-iec-60502-1-061kv-mc-4-sfa/pt-13191/p-55297</t>
+        </is>
+      </c>
+      <c r="I59" t="inlineStr">
+        <is>
+          <t>polycab_lv_power_cable/images/Polycab_LV_Cu_IEC_60502-1_061kV_MC-4_SFA_image.png</t>
+        </is>
+      </c>
       <c r="J59" t="inlineStr">
         <is>
-          <t>polycab_lv_power_cable/brochures/Polycab_LV_AL_IEC_60502-1_061kV_MC-4_SFA_datasheet.pdf</t>
+          <t>polycab_lv_power_cable/brochures/Polycab_LV_Cu_IEC_60502-1_061kV_MC-4_SFA_datasheet.pdf</t>
         </is>
       </c>
       <c r="K59" t="inlineStr">
         <is>
-          <t>Not Found</t>
+          <t>Downloaded</t>
         </is>
       </c>
       <c r="L59" t="inlineStr">
@@ -3320,7 +4108,7 @@
     <row r="60">
       <c r="A60" t="inlineStr">
         <is>
-          <t>Polycab LV IS-7098-I 2C-2XY</t>
+          <t>Polycab LV AL IEC 60502-1 0.6/1kV MC-2 SWA</t>
         </is>
       </c>
       <c r="B60" t="inlineStr">
@@ -3330,31 +4118,47 @@
       </c>
       <c r="C60" t="inlineStr">
         <is>
-          <t>IEC 60502-1, IS 7098-1, BS 5467</t>
+          <t>IEC 60502-1</t>
         </is>
       </c>
       <c r="D60" t="inlineStr">
         <is>
-          <t>CE, BIS, CPRI, FQC</t>
-        </is>
-      </c>
-      <c r="E60" t="inlineStr"/>
-      <c r="F60" t="inlineStr"/>
-      <c r="G60" t="inlineStr"/>
+          <t>CE, FQC</t>
+        </is>
+      </c>
+      <c r="E60" t="inlineStr">
+        <is>
+          <t>Higher dielectric strength, Better electrical, mechanical, And thermal properties, UV resistant, Long service life, Low smoke emission</t>
+        </is>
+      </c>
+      <c r="F60" t="inlineStr">
+        <is>
+          <t>Multi core stranded AL conductor,XLPE/EPR/HEPR insulation, Laid up, Inner covering, Armoured, PVC/Polyethylene/Halogen free Outer sheathed LV Cable sheathed LV Cable</t>
+        </is>
+      </c>
+      <c r="G60" t="inlineStr">
+        <is>
+          <t>Multicore stranded Aluminium, XLPE/EPR/HEPR insulation, Laid up, inner covering,GI wire,PVC/Polyethylene/Halogen free sheathed Cable suitable for fixed installation such as distribution network or industrial installation.These cables are designed for systems with rated AC voltage 1KV (Um=1.2 KV) between two live conductor.</t>
+        </is>
+      </c>
       <c r="H60" t="inlineStr">
         <is>
-          <t>https://polycab.com/polycab-lv-is-7098-i-2c-2xy/pt-13191/p-54740</t>
-        </is>
-      </c>
-      <c r="I60" t="inlineStr"/>
+          <t>https://polycab.com/polycab-lv-al-iec-60502-1-061kv-mc-2-swa/pt-13191/p-55257</t>
+        </is>
+      </c>
+      <c r="I60" t="inlineStr">
+        <is>
+          <t>polycab_lv_power_cable/images/Polycab_LV_AL_IEC_60502-1_061kV_MC-2_SWA_image.png</t>
+        </is>
+      </c>
       <c r="J60" t="inlineStr">
         <is>
-          <t>polycab_lv_power_cable/brochures/Polycab_LV_IS-7098-I_2C-2XY_datasheet.pdf</t>
+          <t>polycab_lv_power_cable/brochures/Polycab_LV_AL_IEC_60502-1_061kV_MC-2_SWA_datasheet.pdf</t>
         </is>
       </c>
       <c r="K60" t="inlineStr">
         <is>
-          <t>Not Found</t>
+          <t>Downloaded</t>
         </is>
       </c>
       <c r="L60" t="inlineStr">
@@ -3366,7 +4170,7 @@
     <row r="61">
       <c r="A61" t="inlineStr">
         <is>
-          <t>Polycab LV IS-7098-I 4C A2XFY</t>
+          <t>Polycab LV IS-7098-I 2C A2XWY</t>
         </is>
       </c>
       <c r="B61" t="inlineStr">
@@ -3376,7 +4180,7 @@
       </c>
       <c r="C61" t="inlineStr">
         <is>
-          <t>IEC 60502-1, IS 7098-1, BS 5467</t>
+          <t>IS 7098-I</t>
         </is>
       </c>
       <c r="D61" t="inlineStr">
@@ -3384,23 +4188,39 @@
           <t>CE, BIS, CPRI, FQC</t>
         </is>
       </c>
-      <c r="E61" t="inlineStr"/>
-      <c r="F61" t="inlineStr"/>
-      <c r="G61" t="inlineStr"/>
+      <c r="E61" t="inlineStr">
+        <is>
+          <t>Higher Current rating, Higher insulation resistance, Better resistance to surge current, Low dielectric losses, Long service life, Higher short circuit rating</t>
+        </is>
+      </c>
+      <c r="F61" t="inlineStr">
+        <is>
+          <t>Two core Aluminium conductor, XLPE Insulation Inner sheathed &amp; GI round armoured &amp; PVC Outer sheathed cable</t>
+        </is>
+      </c>
+      <c r="G61" t="inlineStr">
+        <is>
+          <t>POLYCAB A2XWY MC-2, Stranded compacted aluminium conductor ,XLPE insulated, PVC inner sheathed, Galvanised Steel round wire armour and PVC sheathed confirming to IS 7098-1 is suitable for AC single phase or three phase (earthed or unearthed) systems with rated voltage up to and including 1100 V. This cable is also suitable for DC systems with rated voltage up to and including 1500 V</t>
+        </is>
+      </c>
       <c r="H61" t="inlineStr">
         <is>
-          <t>https://polycab.com/polycab-lv-is-7098-i-4c-a2xfy/pt-13191/p-54728</t>
-        </is>
-      </c>
-      <c r="I61" t="inlineStr"/>
+          <t>https://polycab.com/polycab-lv-is-7098-i-2c-a2xwy/pt-13191/p-54706</t>
+        </is>
+      </c>
+      <c r="I61" t="inlineStr">
+        <is>
+          <t>polycab_lv_power_cable/images/Polycab_LV_IS-7098-I_2C_A2XWY_image.png</t>
+        </is>
+      </c>
       <c r="J61" t="inlineStr">
         <is>
-          <t>polycab_lv_power_cable/brochures/Polycab_LV_IS-7098-I_4C_A2XFY_datasheet.pdf</t>
+          <t>polycab_lv_power_cable/brochures/Polycab_LV_IS-7098-I_2C_A2XWY_datasheet.pdf</t>
         </is>
       </c>
       <c r="K61" t="inlineStr">
         <is>
-          <t>Not Found</t>
+          <t>Downloaded</t>
         </is>
       </c>
       <c r="L61" t="inlineStr">
@@ -3412,7 +4232,7 @@
     <row r="62">
       <c r="A62" t="inlineStr">
         <is>
-          <t>Polycab LV IS-7098-I 3C-A2XY</t>
+          <t>Polycab LV IS-7098-I 2C 2XFY</t>
         </is>
       </c>
       <c r="B62" t="inlineStr">
@@ -3422,7 +4242,7 @@
       </c>
       <c r="C62" t="inlineStr">
         <is>
-          <t>IEC 60502-1, IS 7098-1, BS 5467</t>
+          <t>IS 7098-I</t>
         </is>
       </c>
       <c r="D62" t="inlineStr">
@@ -3430,23 +4250,39 @@
           <t>CE, BIS, CPRI, FQC</t>
         </is>
       </c>
-      <c r="E62" t="inlineStr"/>
-      <c r="F62" t="inlineStr"/>
-      <c r="G62" t="inlineStr"/>
+      <c r="E62" t="inlineStr">
+        <is>
+          <t>Higher Current rating, Higher insulation resistance, Better resistance to surge current, Low dielectric losses, Long service life, Higher short circuit rating</t>
+        </is>
+      </c>
+      <c r="F62" t="inlineStr">
+        <is>
+          <t>Two core copper conductor, XLPE Insulation,PVC Inner sheathed and GI flat armoured and PVC Outer sheathed cable</t>
+        </is>
+      </c>
+      <c r="G62" t="inlineStr">
+        <is>
+          <t>POLYCAB 2XFY MC-2, stranded compacted copper conductor, XLPE insulated, PVC inner sheathed, Galvanised Steel Flat strip armoured, and PVC sheathed confirming to IS 7098-1 is suitable for AC single phase or three phase (earthed or unearthed) systems with rated voltage up to and including 1100 V. This cable is also suitable for DC systems with rated voltage up to and including 1500 V</t>
+        </is>
+      </c>
       <c r="H62" t="inlineStr">
         <is>
-          <t>https://polycab.com/polycab-lv-is-7098-i-3c-a2xy/pt-13191/p-54750</t>
-        </is>
-      </c>
-      <c r="I62" t="inlineStr"/>
+          <t>https://polycab.com/polycab-lv-is-7098-i-2c-2xfy/pt-13191/p-54700</t>
+        </is>
+      </c>
+      <c r="I62" t="inlineStr">
+        <is>
+          <t>polycab_lv_power_cable/images/Polycab_LV_IS-7098-I_2C_2XFY_image.png</t>
+        </is>
+      </c>
       <c r="J62" t="inlineStr">
         <is>
-          <t>polycab_lv_power_cable/brochures/Polycab_LV_IS-7098-I_3C-A2XY_datasheet.pdf</t>
+          <t>polycab_lv_power_cable/brochures/Polycab_LV_IS-7098-I_2C_2XFY_datasheet.pdf</t>
         </is>
       </c>
       <c r="K62" t="inlineStr">
         <is>
-          <t>Not Found</t>
+          <t>Downloaded</t>
         </is>
       </c>
       <c r="L62" t="inlineStr">
@@ -3458,7 +4294,7 @@
     <row r="63">
       <c r="A63" t="inlineStr">
         <is>
-          <t>Polycab LV Cu IEC 60502-1 0.6/1kV MC-3.5 SFA</t>
+          <t>Polycab BS 6724 SC AWA LSZH 0.6/1kV AC</t>
         </is>
       </c>
       <c r="B63" t="inlineStr">
@@ -3468,7 +4304,7 @@
       </c>
       <c r="C63" t="inlineStr">
         <is>
-          <t>IEC 60502-1, BS 5467</t>
+          <t>BS 6724</t>
         </is>
       </c>
       <c r="D63" t="inlineStr">
@@ -3478,25 +4314,37 @@
       </c>
       <c r="E63" t="inlineStr">
         <is>
-          <t>UV Resistant, Low Smoke</t>
-        </is>
-      </c>
-      <c r="F63" t="inlineStr"/>
-      <c r="G63" t="inlineStr"/>
+          <t>Low flame propagation, Low smoke emission, High life, Halogen Free</t>
+        </is>
+      </c>
+      <c r="F63" t="inlineStr">
+        <is>
+          <t>Stranded copper conductor, XLPE/EPR/HEPR Insulated, Extruded Polymeric Bedding, Aluminium round wire armoured, LSZH Outer Sheathed 0.6/1 kV LV cable</t>
+        </is>
+      </c>
+      <c r="G63" t="inlineStr">
+        <is>
+          <t>POLYCAB BS 6724 SC AWA LSZH stranded copper conductor thermosetting material insulated single core Aluminium armoured cable is designed to use for fixed installation in indoor and outdoor power network, underground application, industrial areas and buildings where smoke emission and toxic fumes create a potential risk when exposed to fire.</t>
+        </is>
+      </c>
       <c r="H63" t="inlineStr">
         <is>
-          <t>https://polycab.com/polycab-lv-cu-iec-60502-1-061kv-mc-35-sfa/pt-13191/p-55273</t>
-        </is>
-      </c>
-      <c r="I63" t="inlineStr"/>
+          <t>https://polycab.com/polycab-bs-6724-sc-awa-lszh-061kv-ac/pt-13191/p-55455</t>
+        </is>
+      </c>
+      <c r="I63" t="inlineStr">
+        <is>
+          <t>polycab_lv_power_cable/images/Polycab_BS_6724_SC_AWA_LSZH_061kV_AC_image.png</t>
+        </is>
+      </c>
       <c r="J63" t="inlineStr">
         <is>
-          <t>polycab_lv_power_cable/brochures/Polycab_LV_Cu_IEC_60502-1_061kV_MC-35_SFA_datasheet.pdf</t>
+          <t>polycab_lv_power_cable/brochures/Polycab_BS_6724_SC_AWA_LSZH_061kV_AC_datasheet.pdf</t>
         </is>
       </c>
       <c r="K63" t="inlineStr">
         <is>
-          <t>Not Found</t>
+          <t>Downloaded</t>
         </is>
       </c>
       <c r="L63" t="inlineStr">

</xml_diff>